<commit_message>
replaced all reading times with average
</commit_message>
<xml_diff>
--- a/model-inference/decisionTree/experiments/gpu_results/airline_classification/airline.xlsx
+++ b/model-inference/decisionTree/experiments/gpu_results/airline_classification/airline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\11\netsdb\model-inference\decisionTree\experiments\gpu_results\airline_classification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4392492-0A8D-473B-B40D-D50A784F2A35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C612717-4F63-45AE-9F2C-600EB3DF061F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5988" yWindow="-372" windowWidth="17280" windowHeight="8964" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="10_trees" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="593" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="32">
   <si>
     <t>query size</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>CPU</t>
+  </si>
+  <si>
+    <t>average</t>
   </si>
 </sst>
 </file>
@@ -2962,13 +2965,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>46.588900089263817</c:v>
+                  <c:v>46.337956744592212</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>87.255288362502895</c:v>
+                  <c:v>86.640738088052302</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>178.33080959320031</c:v>
+                  <c:v>178.3245092214749</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3086,13 +3089,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>46.957735776901124</c:v>
+                  <c:v>46.727786857049516</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>71.86143803596481</c:v>
+                  <c:v>71.659197884957791</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>127.31808519363391</c:v>
+                  <c:v>127.19957955495599</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3210,13 +3213,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>45.945363283157256</c:v>
+                  <c:v>45.942891198556445</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53.451896667480419</c:v>
+                  <c:v>53.154491740625012</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>72.432852029800202</c:v>
+                  <c:v>72.36979134694819</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3334,13 +3337,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>44.644665479660013</c:v>
+                  <c:v>44.458604413430805</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45.118538618087669</c:v>
+                  <c:v>45.215932208459478</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57.542337894439626</c:v>
+                  <c:v>57.993606406610112</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3630,7 +3633,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>final!$G$2</c15:sqref>
@@ -3690,7 +3693,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -3712,7 +3715,7 @@
                 </c:dLbls>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>final!$A$3:$A$5</c15:sqref>
@@ -3736,7 +3739,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>final!$G$3:$G$5</c15:sqref>
@@ -3749,7 +3752,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-E33F-427B-B675-8BF78811A0DF}"/>
                   </c:ext>
@@ -4125,13 +4128,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>45.822473049163719</c:v>
+                  <c:v>46.461994248788429</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85.755883693694898</c:v>
+                  <c:v>86.128751832406479</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>176.60673642158417</c:v>
+                  <c:v>176.6493080438774</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4249,13 +4252,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>46.728768348693684</c:v>
+                  <c:v>46.581592399041675</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>72.449626445770107</c:v>
+                  <c:v>71.787981826226698</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>125.5527627468108</c:v>
+                  <c:v>125.79967578069449</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4373,13 +4376,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>45.9850335121154</c:v>
+                  <c:v>46.214565116326888</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>52.779498338699256</c:v>
+                  <c:v>52.620731192987037</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69.724192857742196</c:v>
+                  <c:v>69.340525227944894</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4497,13 +4500,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>43.574426651000877</c:v>
+                  <c:v>44.141585904519673</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43.132436513900679</c:v>
+                  <c:v>43.034369307916272</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47.603817701339644</c:v>
+                  <c:v>47.262526828210461</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4621,13 +4624,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>49.247249603271371</c:v>
+                  <c:v>49.288450557153269</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53.278722286224301</c:v>
+                  <c:v>53.245069819848602</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>59.234944820403904</c:v>
+                  <c:v>58.540425855081082</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5285,13 +5288,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>45.443762540817097</c:v>
+                  <c:v>46.245139199655085</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>85.861827135085903</c:v>
+                  <c:v>86.201553183953791</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>176.50412893295251</c:v>
+                  <c:v>177.0484917940305</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5409,13 +5412,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>46.475845575332549</c:v>
+                  <c:v>46.370733577172842</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>73.0877263545988</c:v>
+                  <c:v>72.195126372735487</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>127.6398167610167</c:v>
+                  <c:v>126.88626487867118</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5533,13 +5536,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>45.567111015319696</c:v>
+                  <c:v>46.223801452081275</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53.220368623733449</c:v>
+                  <c:v>52.516989308755441</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>68.829155921935808</c:v>
+                  <c:v>69.309853869836289</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5657,13 +5660,13 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>42.292098522186251</c:v>
+                  <c:v>42.219190198342915</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>45.928158044815014</c:v>
+                  <c:v>45.447910148065205</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55.264179706573401</c:v>
+                  <c:v>54.939173537652586</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5953,7 +5956,7 @@
                 <c:order val="5"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>final!$G$14</c15:sqref>
@@ -6013,7 +6016,7 @@
                   <c:showPercent val="0"/>
                   <c:showBubbleSize val="0"/>
                   <c:showLeaderLines val="0"/>
-                  <c:extLst>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                     <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                       <c15:showLeaderLines val="1"/>
                       <c15:leaderLines>
@@ -6035,7 +6038,7 @@
                 </c:dLbls>
                 <c:cat>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>final!$A$15:$A$17</c15:sqref>
@@ -6059,7 +6062,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>final!$G$15:$G$17</c15:sqref>
@@ -6072,7 +6075,7 @@
                     </c:numCache>
                   </c:numRef>
                 </c:val>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000005-081F-44EE-B8FA-BD5FDC5849E3}"/>
                   </c:ext>
@@ -10007,10 +10010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L103"/>
+  <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8:L13"/>
+    <sheetView topLeftCell="A94" workbookViewId="0">
+      <selection activeCell="K110" sqref="K110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10088,12 +10091,12 @@
         <v>226307.79361724801</v>
       </c>
       <c r="K2">
-        <f>SUM(E2,G2,H2)</f>
-        <v>251089.59341049119</v>
+        <f>SUM($E$105,G2,H2)</f>
+        <v>250646.43152372059</v>
       </c>
       <c r="L2">
         <f>PRODUCT(K2,0.001)</f>
-        <v>251.0895934104912</v>
+        <v>250.64643152372059</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -10128,12 +10131,12 @@
         <v>37441.178798675501</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K66" si="0">SUM(E3,G3,H3)</f>
-        <v>65756.805658340309</v>
+        <f t="shared" ref="K3:K66" si="0">SUM($E$105,G3,H3)</f>
+        <v>65756.842452447396</v>
       </c>
       <c r="L3">
         <f t="shared" ref="L3:L66" si="1">PRODUCT(K3,0.001)</f>
-        <v>65.756805658340312</v>
+        <v>65.756842452447401</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -10169,11 +10172,11 @@
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>48338.52672576897</v>
+        <v>48580.394107263157</v>
       </c>
       <c r="L4">
         <f t="shared" si="1"/>
-        <v>48.338526725768972</v>
+        <v>48.58039410726316</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -10209,11 +10212,11 @@
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>46588.900089263814</v>
+        <v>46337.956744592208</v>
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>46.588900089263817</v>
+        <v>46.337956744592212</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -10249,11 +10252,11 @@
       </c>
       <c r="K6">
         <f t="shared" si="0"/>
-        <v>47162.418127059813</v>
+        <v>46860.516387383999</v>
       </c>
       <c r="L6">
         <f t="shared" si="1"/>
-        <v>47.162418127059816</v>
+        <v>46.860516387384003</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.3">
@@ -10289,11 +10292,11 @@
       </c>
       <c r="K7">
         <f t="shared" si="0"/>
-        <v>48845.138549804622</v>
+        <v>47673.016148965413</v>
       </c>
       <c r="L7">
         <f t="shared" si="1"/>
-        <v>48.845138549804624</v>
+        <v>47.673016148965417</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -10329,11 +10332,11 @@
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>176566.96677207929</v>
+        <v>176349.50431005241</v>
       </c>
       <c r="L8">
         <f t="shared" si="1"/>
-        <v>176.5669667720793</v>
+        <v>176.3495043100524</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -10369,11 +10372,11 @@
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>59334.0828418729</v>
+        <v>60201.814490716388</v>
       </c>
       <c r="L9">
         <f t="shared" si="1"/>
-        <v>59.334082841872899</v>
+        <v>60.201814490716387</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -10409,11 +10412,11 @@
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>47882.322072982708</v>
+        <v>47698.751527230801</v>
       </c>
       <c r="L10">
         <f t="shared" si="1"/>
-        <v>47.88232207298271</v>
+        <v>47.698751527230804</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -10449,11 +10452,11 @@
       </c>
       <c r="K11">
         <f t="shared" si="0"/>
-        <v>47615.296840667681</v>
+        <v>47398.978549401872</v>
       </c>
       <c r="L11">
         <f t="shared" si="1"/>
-        <v>47.615296840667682</v>
+        <v>47.398978549401875</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.3">
@@ -10489,11 +10492,11 @@
       </c>
       <c r="K12">
         <f t="shared" si="0"/>
-        <v>46957.735776901121</v>
+        <v>46727.786857049512</v>
       </c>
       <c r="L12">
         <f t="shared" si="1"/>
-        <v>46.957735776901124</v>
+        <v>46.727786857049516</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -10529,11 +10532,11 @@
       </c>
       <c r="K13">
         <f t="shared" si="0"/>
-        <v>47711.446762084925</v>
+        <v>47430.650073449709</v>
       </c>
       <c r="L13">
         <f t="shared" si="1"/>
-        <v>47.711446762084925</v>
+        <v>47.430650073449712</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -10569,11 +10572,11 @@
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>72124.968528747399</v>
+        <v>71778.416234414588</v>
       </c>
       <c r="L14">
         <f t="shared" si="1"/>
-        <v>72.124968528747402</v>
+        <v>71.778416234414593</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -10609,11 +10612,11 @@
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>57517.668485641305</v>
+        <v>57198.877650659095</v>
       </c>
       <c r="L15">
         <f t="shared" si="1"/>
-        <v>57.517668485641309</v>
+        <v>57.198877650659099</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -10649,11 +10652,11 @@
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>57278.313875198204</v>
+        <v>57088.843423287894</v>
       </c>
       <c r="L16">
         <f t="shared" si="1"/>
-        <v>57.278313875198208</v>
+        <v>57.088843423287898</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -10689,11 +10692,11 @@
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>52540.710210800156</v>
+        <v>53354.193765084856</v>
       </c>
       <c r="L17">
         <f t="shared" si="1"/>
-        <v>52.540710210800157</v>
+        <v>53.354193765084858</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -10729,11 +10732,11 @@
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
-        <v>56173.669576644796</v>
+        <v>56745.691615502888</v>
       </c>
       <c r="L18">
         <f t="shared" si="1"/>
-        <v>56.173669576644798</v>
+        <v>56.745691615502892</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -10769,11 +10772,11 @@
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>57337.4712467192</v>
+        <v>58146.331149499383</v>
       </c>
       <c r="L19">
         <f t="shared" si="1"/>
-        <v>57.337471246719204</v>
+        <v>58.146331149499382</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -10809,11 +10812,11 @@
       </c>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>108208.05597305291</v>
+        <v>108153.89497892148</v>
       </c>
       <c r="L20">
         <f t="shared" si="1"/>
-        <v>108.20805597305291</v>
+        <v>108.15389497892149</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -10849,11 +10852,11 @@
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>53006.514549255291</v>
+        <v>53605.579215447979</v>
       </c>
       <c r="L21">
         <f t="shared" si="1"/>
-        <v>53.006514549255293</v>
+        <v>53.605579215447982</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -10889,11 +10892,11 @@
       </c>
       <c r="K22">
         <f t="shared" si="0"/>
-        <v>48842.433929443192</v>
+        <v>48771.59555570368</v>
       </c>
       <c r="L22">
         <f t="shared" si="1"/>
-        <v>48.842433929443196</v>
+        <v>48.771595555703684</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -10929,11 +10932,11 @@
       </c>
       <c r="K23">
         <f t="shared" si="0"/>
-        <v>46147.973775863589</v>
+        <v>46190.157014291377</v>
       </c>
       <c r="L23">
         <f t="shared" si="1"/>
-        <v>46.147973775863591</v>
+        <v>46.19015701429138</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -10969,11 +10972,11 @@
       </c>
       <c r="K24">
         <f t="shared" si="0"/>
-        <v>46101.127862930167</v>
+        <v>46239.00230542905</v>
       </c>
       <c r="L24">
         <f t="shared" si="1"/>
-        <v>46.10112786293017</v>
+        <v>46.239002305429054</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -11009,11 +11012,11 @@
       </c>
       <c r="K25">
         <f t="shared" si="0"/>
-        <v>45945.363283157254</v>
+        <v>45942.891198556441</v>
       </c>
       <c r="L25">
         <f t="shared" si="1"/>
-        <v>45.945363283157256</v>
+        <v>45.942891198556445</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -11049,11 +11052,11 @@
       </c>
       <c r="K26">
         <f t="shared" si="0"/>
-        <v>152601.80020332246</v>
+        <v>153305.25429860756</v>
       </c>
       <c r="L26">
         <f t="shared" si="1"/>
-        <v>152.60180020332245</v>
+        <v>153.30525429860757</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -11089,11 +11092,11 @@
       </c>
       <c r="K27">
         <f t="shared" si="0"/>
-        <v>52910.030841827349</v>
+        <v>53843.633014123538</v>
       </c>
       <c r="L27">
         <f t="shared" si="1"/>
-        <v>52.91003084182735</v>
+        <v>53.84363301412354</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -11129,11 +11132,11 @@
       </c>
       <c r="K28">
         <f t="shared" si="0"/>
-        <v>45198.522806167559</v>
+        <v>45860.200244348147</v>
       </c>
       <c r="L28">
         <f t="shared" si="1"/>
-        <v>45.19852280616756</v>
+        <v>45.86020024434815</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
@@ -11169,11 +11172,11 @@
       </c>
       <c r="K29">
         <f t="shared" si="0"/>
-        <v>44644.665479660012</v>
+        <v>44458.604413430803</v>
       </c>
       <c r="L29">
         <f t="shared" si="1"/>
-        <v>44.644665479660013</v>
+        <v>44.458604413430805</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -11209,11 +11212,11 @@
       </c>
       <c r="K30">
         <f t="shared" si="0"/>
-        <v>45092.133998870813</v>
+        <v>44580.82755224</v>
       </c>
       <c r="L30">
         <f t="shared" si="1"/>
-        <v>45.092133998870814</v>
+        <v>44.580827552240002</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -11249,11 +11252,11 @@
       </c>
       <c r="K31">
         <f t="shared" si="0"/>
-        <v>46667.626380920308</v>
+        <v>46576.528865258799</v>
       </c>
       <c r="L31">
         <f t="shared" si="1"/>
-        <v>46.667626380920311</v>
+        <v>46.576528865258801</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -11289,11 +11292,11 @@
       </c>
       <c r="K32">
         <f t="shared" si="0"/>
-        <v>263432.8756332394</v>
+        <v>263398.04943219875</v>
       </c>
       <c r="L32">
         <f t="shared" si="1"/>
-        <v>263.43287563323941</v>
+        <v>263.39804943219877</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -11329,11 +11332,11 @@
       </c>
       <c r="K33">
         <f t="shared" si="0"/>
-        <v>67683.781147002999</v>
+        <v>67504.928666512991</v>
       </c>
       <c r="L33">
         <f t="shared" si="1"/>
-        <v>67.683781147003003</v>
+        <v>67.504928666512996</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -11369,11 +11372,11 @@
       </c>
       <c r="K34">
         <f t="shared" si="0"/>
-        <v>48548.031330108497</v>
+        <v>48500.170308511289</v>
       </c>
       <c r="L34">
         <f t="shared" si="1"/>
-        <v>48.5480313301085</v>
+        <v>48.500170308511294</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -11409,11 +11412,11 @@
       </c>
       <c r="K35">
         <f t="shared" si="0"/>
-        <v>46831.551551818688</v>
+        <v>47374.376613061482</v>
       </c>
       <c r="L35">
         <f t="shared" si="1"/>
-        <v>46.831551551818691</v>
+        <v>47.374376613061486</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -11449,11 +11452,11 @@
       </c>
       <c r="K36">
         <f t="shared" si="0"/>
-        <v>45822.473049163716</v>
+        <v>46755.893784921209</v>
       </c>
       <c r="L36">
         <f t="shared" si="1"/>
-        <v>45.822473049163719</v>
+        <v>46.755893784921213</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.3">
@@ -11489,11 +11492,11 @@
       </c>
       <c r="K37">
         <f t="shared" si="0"/>
-        <v>45865.183115005442</v>
+        <v>46461.994248788425</v>
       </c>
       <c r="L37">
         <f t="shared" si="1"/>
-        <v>45.865183115005443</v>
+        <v>46.461994248788429</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -11529,11 +11532,11 @@
       </c>
       <c r="K38">
         <f t="shared" si="0"/>
-        <v>184787.06598281761</v>
+        <v>184888.12835828459</v>
       </c>
       <c r="L38">
         <f t="shared" si="1"/>
-        <v>184.78706598281761</v>
+        <v>184.8881283582846</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -11569,11 +11572,11 @@
       </c>
       <c r="K39">
         <f t="shared" si="0"/>
-        <v>62363.6898994445</v>
+        <v>62163.836079995686</v>
       </c>
       <c r="L39">
         <f t="shared" si="1"/>
-        <v>62.363689899444502</v>
+        <v>62.16383607999569</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -11609,11 +11612,11 @@
       </c>
       <c r="K40">
         <f t="shared" si="0"/>
-        <v>48800.031185150016</v>
+        <v>48663.886147897298</v>
       </c>
       <c r="L40">
         <f t="shared" si="1"/>
-        <v>48.800031185150019</v>
+        <v>48.663886147897301</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
@@ -11649,11 +11652,11 @@
       </c>
       <c r="K41">
         <f t="shared" si="0"/>
-        <v>47328.0134201049</v>
+        <v>47122.400838296489</v>
       </c>
       <c r="L41">
         <f t="shared" si="1"/>
-        <v>47.328013420104902</v>
+        <v>47.122400838296493</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.3">
@@ -11689,11 +11692,11 @@
       </c>
       <c r="K42">
         <f t="shared" si="0"/>
-        <v>47470.44563293449</v>
+        <v>47313.177424829082</v>
       </c>
       <c r="L42">
         <f t="shared" si="1"/>
-        <v>47.470445632934492</v>
+        <v>47.313177424829085</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
@@ -11729,11 +11732,11 @@
       </c>
       <c r="K43">
         <f t="shared" si="0"/>
-        <v>46728.76834869368</v>
+        <v>46581.59239904167</v>
       </c>
       <c r="L43">
         <f t="shared" si="1"/>
-        <v>46.728768348693684</v>
+        <v>46.581592399041675</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
@@ -11769,11 +11772,11 @@
       </c>
       <c r="K44">
         <f t="shared" si="0"/>
-        <v>69501.665115356402</v>
+        <v>69903.942901055882</v>
       </c>
       <c r="L44">
         <f t="shared" si="1"/>
-        <v>69.501665115356403</v>
+        <v>69.903942901055885</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
@@ -11809,11 +11812,11 @@
       </c>
       <c r="K45">
         <f t="shared" si="0"/>
-        <v>59359.628438949396</v>
+        <v>59610.426741998184</v>
       </c>
       <c r="L45">
         <f t="shared" si="1"/>
-        <v>59.3596284389494</v>
+        <v>59.610426741998182</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -11849,11 +11852,11 @@
       </c>
       <c r="K46">
         <f t="shared" si="0"/>
-        <v>55490.199565887197</v>
+        <v>56318.05856839889</v>
       </c>
       <c r="L46">
         <f t="shared" si="1"/>
-        <v>55.490199565887195</v>
+        <v>56.318058568398889</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -11889,11 +11892,11 @@
       </c>
       <c r="K47">
         <f t="shared" si="0"/>
-        <v>56264.9939060209</v>
+        <v>56447.99883977649</v>
       </c>
       <c r="L47">
         <f t="shared" si="1"/>
-        <v>56.264993906020898</v>
+        <v>56.447998839776488</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
@@ -11929,11 +11932,11 @@
       </c>
       <c r="K48">
         <f t="shared" si="0"/>
-        <v>57232.923269271698</v>
+        <v>58146.210748116988</v>
       </c>
       <c r="L48">
         <f t="shared" si="1"/>
-        <v>57.232923269271701</v>
+        <v>58.146210748116992</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
@@ -11969,11 +11972,11 @@
       </c>
       <c r="K49">
         <f t="shared" si="0"/>
-        <v>57740.967273711998</v>
+        <v>58596.265155236688</v>
       </c>
       <c r="L49">
         <f t="shared" si="1"/>
-        <v>57.740967273712002</v>
+        <v>58.596265155236686</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
@@ -12009,11 +12012,11 @@
       </c>
       <c r="K50">
         <f t="shared" si="0"/>
-        <v>107184.84568595869</v>
+        <v>108116.18145124198</v>
       </c>
       <c r="L50">
         <f t="shared" si="1"/>
-        <v>107.18484568595869</v>
+        <v>108.11618145124199</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
@@ -12049,11 +12052,11 @@
       </c>
       <c r="K51">
         <f t="shared" si="0"/>
-        <v>51735.850095748843</v>
+        <v>52616.488295953328</v>
       </c>
       <c r="L51">
         <f t="shared" si="1"/>
-        <v>51.735850095748845</v>
+        <v>52.616488295953332</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -12089,11 +12092,11 @@
       </c>
       <c r="K52">
         <f t="shared" si="0"/>
-        <v>47283.551692962581</v>
+        <v>48165.051537911968</v>
       </c>
       <c r="L52">
         <f t="shared" si="1"/>
-        <v>47.283551692962583</v>
+        <v>48.165051537911971</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -12129,11 +12132,11 @@
       </c>
       <c r="K53">
         <f t="shared" si="0"/>
-        <v>47431.65445327753</v>
+        <v>48068.691808145115</v>
       </c>
       <c r="L53">
         <f t="shared" si="1"/>
-        <v>47.431654453277531</v>
+        <v>48.068691808145118</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -12169,11 +12172,11 @@
       </c>
       <c r="K54">
         <f t="shared" si="0"/>
-        <v>45985.033512115398</v>
+        <v>46214.565116326885</v>
       </c>
       <c r="L54">
         <f t="shared" si="1"/>
-        <v>45.9850335121154</v>
+        <v>46.214565116326888</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
@@ -12209,11 +12212,11 @@
       </c>
       <c r="K55">
         <f t="shared" si="0"/>
-        <v>46113.296270370367</v>
+        <v>46398.11618940116</v>
       </c>
       <c r="L55">
         <f t="shared" si="1"/>
-        <v>46.11329627037037</v>
+        <v>46.398116189401158</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.3">
@@ -12249,11 +12252,11 @@
       </c>
       <c r="K56">
         <f t="shared" si="0"/>
-        <v>155482.83267021162</v>
+        <v>155086.76393644093</v>
       </c>
       <c r="L56">
         <f t="shared" si="1"/>
-        <v>155.48283267021162</v>
+        <v>155.08676393644092</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
@@ -12289,11 +12292,11 @@
       </c>
       <c r="K57">
         <f t="shared" si="0"/>
-        <v>52884.964227676319</v>
+        <v>52824.864703576604</v>
       </c>
       <c r="L57">
         <f t="shared" si="1"/>
-        <v>52.884964227676321</v>
+        <v>52.824864703576608</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
@@ -12329,11 +12332,11 @@
       </c>
       <c r="K58">
         <f t="shared" si="0"/>
-        <v>43937.707901000882</v>
+        <v>44566.074448983767</v>
       </c>
       <c r="L58">
         <f t="shared" si="1"/>
-        <v>43.937707901000884</v>
+        <v>44.56607444898377</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -12369,11 +12372,11 @@
       </c>
       <c r="K59">
         <f t="shared" si="0"/>
-        <v>43574.426651000875</v>
+        <v>44247.165280740359</v>
       </c>
       <c r="L59">
         <f t="shared" si="1"/>
-        <v>43.574426651000877</v>
+        <v>44.247165280740361</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
@@ -12409,11 +12412,11 @@
       </c>
       <c r="K60">
         <f t="shared" si="0"/>
-        <v>44077.377796173081</v>
+        <v>44141.58590451967</v>
       </c>
       <c r="L60">
         <f t="shared" si="1"/>
-        <v>44.077377796173081</v>
+        <v>44.141585904519673</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
@@ -12449,11 +12452,11 @@
       </c>
       <c r="K61">
         <f t="shared" si="0"/>
-        <v>44845.692396163911</v>
+        <v>44186.662513177493</v>
       </c>
       <c r="L61">
         <f t="shared" si="1"/>
-        <v>44.845692396163912</v>
+        <v>44.186662513177495</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
@@ -12489,11 +12492,11 @@
       </c>
       <c r="K62">
         <f t="shared" si="0"/>
-        <v>375965.71326255705</v>
+        <v>375906.19285718602</v>
       </c>
       <c r="L62">
         <f t="shared" si="1"/>
-        <v>375.96571326255707</v>
+        <v>375.906192857186</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
@@ -12529,11 +12532,11 @@
       </c>
       <c r="K63">
         <f t="shared" si="0"/>
-        <v>84847.905874252203</v>
+        <v>84522.126513879397</v>
       </c>
       <c r="L63">
         <f t="shared" si="1"/>
-        <v>84.847905874252206</v>
+        <v>84.5221265138794</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
@@ -12569,11 +12572,11 @@
       </c>
       <c r="K64">
         <f t="shared" si="0"/>
-        <v>55815.5820369719</v>
+        <v>55243.265468041885</v>
       </c>
       <c r="L64">
         <f t="shared" si="1"/>
-        <v>55.815582036971904</v>
+        <v>55.243265468041884</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
@@ -12609,11 +12612,11 @@
       </c>
       <c r="K65">
         <f t="shared" si="0"/>
-        <v>52733.16574096668</v>
+        <v>52566.50312558897</v>
       </c>
       <c r="L65">
         <f t="shared" si="1"/>
-        <v>52.733165740966683</v>
+        <v>52.566503125588973</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
@@ -12649,11 +12652,11 @@
       </c>
       <c r="K66">
         <f t="shared" si="0"/>
-        <v>52126.939296722281</v>
+        <v>52448.099929254066</v>
       </c>
       <c r="L66">
         <f t="shared" si="1"/>
-        <v>52.126939296722284</v>
+        <v>52.448099929254063</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
@@ -12688,12 +12691,12 @@
         <v>21590.205907821601</v>
       </c>
       <c r="K67">
-        <f t="shared" ref="K67:K103" si="2">SUM(E67,G67,H67)</f>
-        <v>53877.621412277134</v>
+        <f t="shared" ref="K67:K103" si="2">SUM($E$105,G67,H67)</f>
+        <v>53891.822177331531</v>
       </c>
       <c r="L67">
         <f t="shared" ref="L67:L103" si="3">PRODUCT(K67,0.001)</f>
-        <v>53.877621412277136</v>
+        <v>53.891822177331534</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
@@ -12729,11 +12732,11 @@
       </c>
       <c r="K68">
         <f t="shared" si="2"/>
-        <v>421119.9557781216</v>
+        <v>420686.69541494106</v>
       </c>
       <c r="L68">
         <f t="shared" si="3"/>
-        <v>421.11995577812161</v>
+        <v>420.68669541494108</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
@@ -12769,11 +12772,11 @@
       </c>
       <c r="K69">
         <f t="shared" si="2"/>
-        <v>85239.433288574204</v>
+        <v>86096.481162469485</v>
       </c>
       <c r="L69">
         <f t="shared" si="3"/>
-        <v>85.239433288574205</v>
+        <v>86.096481162469487</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
@@ -12809,11 +12812,11 @@
       </c>
       <c r="K70">
         <f t="shared" si="2"/>
-        <v>53917.721509933421</v>
+        <v>53601.676303308108</v>
       </c>
       <c r="L70">
         <f t="shared" si="3"/>
-        <v>53.917721509933422</v>
+        <v>53.601676303308111</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
@@ -12849,11 +12852,11 @@
       </c>
       <c r="K71">
         <f t="shared" si="2"/>
-        <v>49247.249603271368</v>
+        <v>49288.450557153265</v>
       </c>
       <c r="L71">
         <f t="shared" si="3"/>
-        <v>49.247249603271371</v>
+        <v>49.288450557153269</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
@@ -12889,11 +12892,11 @@
       </c>
       <c r="K72">
         <f t="shared" si="2"/>
-        <v>50704.333066940279</v>
+        <v>50390.247661035173</v>
       </c>
       <c r="L72">
         <f t="shared" si="3"/>
-        <v>50.704333066940279</v>
+        <v>50.390247661035175</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
@@ -12929,11 +12932,11 @@
       </c>
       <c r="K73">
         <f t="shared" si="2"/>
-        <v>51374.229669570814</v>
+        <v>51157.00729505311</v>
       </c>
       <c r="L73">
         <f t="shared" si="3"/>
-        <v>51.374229669570816</v>
+        <v>51.157007295053113</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
@@ -12969,11 +12972,11 @@
       </c>
       <c r="K74">
         <f t="shared" si="2"/>
-        <v>262546.16260528518</v>
+        <v>262584.64749471401</v>
       </c>
       <c r="L74">
         <f t="shared" si="3"/>
-        <v>262.54616260528519</v>
+        <v>262.58464749471403</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
@@ -13009,11 +13012,11 @@
       </c>
       <c r="K75">
         <f t="shared" si="2"/>
-        <v>68188.627719879005</v>
+        <v>67811.25410215139</v>
       </c>
       <c r="L75">
         <f t="shared" si="3"/>
-        <v>68.188627719879008</v>
+        <v>67.811254102151395</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
@@ -13049,11 +13052,11 @@
       </c>
       <c r="K76">
         <f t="shared" si="2"/>
-        <v>49353.396892547535</v>
+        <v>49006.919700067127</v>
       </c>
       <c r="L76">
         <f t="shared" si="3"/>
-        <v>49.353396892547536</v>
+        <v>49.006919700067129</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
@@ -13089,11 +13092,11 @@
       </c>
       <c r="K77">
         <f t="shared" si="2"/>
-        <v>45922.23238945</v>
+        <v>46543.939429681392</v>
       </c>
       <c r="L77">
         <f t="shared" si="3"/>
-        <v>45.922232389450002</v>
+        <v>46.543939429681394</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
@@ -13129,11 +13132,11 @@
       </c>
       <c r="K78">
         <f t="shared" si="2"/>
-        <v>47726.667404174688</v>
+        <v>48597.19594136958</v>
       </c>
       <c r="L78">
         <f t="shared" si="3"/>
-        <v>47.726667404174691</v>
+        <v>48.597195941369584</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.3">
@@ -13169,11 +13172,11 @@
       </c>
       <c r="K79">
         <f t="shared" si="2"/>
-        <v>45443.762540817093</v>
+        <v>46245.139199655081</v>
       </c>
       <c r="L79">
         <f t="shared" si="3"/>
-        <v>45.443762540817097</v>
+        <v>46.245139199655085</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
@@ -13209,11 +13212,11 @@
       </c>
       <c r="K80">
         <f t="shared" si="2"/>
-        <v>186117.36059188822</v>
+        <v>186025.06025449513</v>
       </c>
       <c r="L80">
         <f t="shared" si="3"/>
-        <v>186.11736059188823</v>
+        <v>186.02506025449512</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
@@ -13249,11 +13252,11 @@
       </c>
       <c r="K81">
         <f t="shared" si="2"/>
-        <v>62166.291952132997</v>
+        <v>61998.116570870887</v>
       </c>
       <c r="L81">
         <f t="shared" si="3"/>
-        <v>62.166291952133001</v>
+        <v>61.998116570870891</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
@@ -13289,11 +13292,11 @@
       </c>
       <c r="K82">
         <f t="shared" si="2"/>
-        <v>49029.103517532174</v>
+        <v>48634.143191735755</v>
       </c>
       <c r="L82">
         <f t="shared" si="3"/>
-        <v>49.029103517532178</v>
+        <v>48.634143191735753</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
@@ -13329,11 +13332,11 @@
       </c>
       <c r="K83">
         <f t="shared" si="2"/>
-        <v>47649.396896362203</v>
+        <v>47034.132319848592</v>
       </c>
       <c r="L83">
         <f t="shared" si="3"/>
-        <v>47.649396896362205</v>
+        <v>47.034132319848595</v>
       </c>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
@@ -13369,11 +13372,11 @@
       </c>
       <c r="K84">
         <f t="shared" si="2"/>
-        <v>47706.413507461417</v>
+        <v>47178.138095300208</v>
       </c>
       <c r="L84">
         <f t="shared" si="3"/>
-        <v>47.70641350746142</v>
+        <v>47.178138095300206</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.3">
@@ -13409,11 +13412,11 @@
       </c>
       <c r="K85">
         <f t="shared" si="2"/>
-        <v>46475.845575332547</v>
+        <v>46370.733577172839</v>
       </c>
       <c r="L85">
         <f t="shared" si="3"/>
-        <v>46.475845575332549</v>
+        <v>46.370733577172842</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.3">
@@ -13449,11 +13452,11 @@
       </c>
       <c r="K86">
         <f t="shared" si="2"/>
-        <v>74141.060829162394</v>
+        <v>74507.758933465491</v>
       </c>
       <c r="L86">
         <f t="shared" si="3"/>
-        <v>74.141060829162399</v>
+        <v>74.507758933465496</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
@@ -13489,11 +13492,11 @@
       </c>
       <c r="K87">
         <f t="shared" si="2"/>
-        <v>54982.385396957303</v>
+        <v>55443.492251794392</v>
       </c>
       <c r="L87">
         <f t="shared" si="3"/>
-        <v>54.982385396957305</v>
+        <v>55.443492251794396</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
@@ -13529,11 +13532,11 @@
       </c>
       <c r="K88">
         <f t="shared" si="2"/>
-        <v>54085.4628086089</v>
+        <v>54323.229867379683</v>
       </c>
       <c r="L88">
         <f t="shared" si="3"/>
-        <v>54.085462808608902</v>
+        <v>54.323229867379688</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
@@ -13569,11 +13572,11 @@
       </c>
       <c r="K89">
         <f t="shared" si="2"/>
-        <v>56830.123662948507</v>
+        <v>56429.171878259192</v>
       </c>
       <c r="L89">
         <f t="shared" si="3"/>
-        <v>56.830123662948509</v>
+        <v>56.429171878259197</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
@@ -13609,11 +13612,11 @@
       </c>
       <c r="K90">
         <f t="shared" si="2"/>
-        <v>57130.544185638297</v>
+        <v>58089.371997277791</v>
       </c>
       <c r="L90">
         <f t="shared" si="3"/>
-        <v>57.1305441856383</v>
+        <v>58.089371997277794</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
@@ -13649,11 +13652,11 @@
       </c>
       <c r="K91">
         <f t="shared" si="2"/>
-        <v>57883.382320403995</v>
+        <v>58551.20523587949</v>
       </c>
       <c r="L91">
         <f t="shared" si="3"/>
-        <v>57.883382320403996</v>
+        <v>58.551205235879493</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
@@ -13689,11 +13692,11 @@
       </c>
       <c r="K92">
         <f t="shared" si="2"/>
-        <v>108861.81402206401</v>
+        <v>109522.00897351978</v>
       </c>
       <c r="L92">
         <f t="shared" si="3"/>
-        <v>108.86181402206401</v>
+        <v>109.52200897351979</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
@@ -13729,11 +13732,11 @@
       </c>
       <c r="K93">
         <f t="shared" si="2"/>
-        <v>52623.225212096993</v>
+        <v>53460.521537225279</v>
       </c>
       <c r="L93">
         <f t="shared" si="3"/>
-        <v>52.623225212096997</v>
+        <v>53.460521537225283</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
@@ -13769,11 +13772,11 @@
       </c>
       <c r="K94">
         <f t="shared" si="2"/>
-        <v>47814.136505126822</v>
+        <v>48258.426505487005</v>
       </c>
       <c r="L94">
         <f t="shared" si="3"/>
-        <v>47.814136505126825</v>
+        <v>48.258426505487009</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
@@ -13809,11 +13812,11 @@
       </c>
       <c r="K95">
         <f t="shared" si="2"/>
-        <v>45567.111015319693</v>
+        <v>46223.801452081272</v>
       </c>
       <c r="L95">
         <f t="shared" si="3"/>
-        <v>45.567111015319696</v>
+        <v>46.223801452081275</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
@@ -13849,11 +13852,11 @@
       </c>
       <c r="K96">
         <f t="shared" si="2"/>
-        <v>47224.130630493077</v>
+        <v>46591.526585977168</v>
       </c>
       <c r="L96">
         <f t="shared" si="3"/>
-        <v>47.224130630493079</v>
+        <v>46.591526585977171</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
@@ -13889,11 +13892,11 @@
       </c>
       <c r="K97">
         <f t="shared" si="2"/>
-        <v>47477.331161498892</v>
+        <v>47502.927619378577</v>
       </c>
       <c r="L97">
         <f t="shared" si="3"/>
-        <v>47.477331161498896</v>
+        <v>47.502927619378575</v>
       </c>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.3">
@@ -13929,11 +13932,11 @@
       </c>
       <c r="K98">
         <f t="shared" si="2"/>
-        <v>153505.54156303304</v>
+        <v>153462.60769979152</v>
       </c>
       <c r="L98">
         <f t="shared" si="3"/>
-        <v>153.50554156303303</v>
+        <v>153.46260769979153</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
@@ -13969,11 +13972,11 @@
       </c>
       <c r="K99">
         <f t="shared" si="2"/>
-        <v>55587.491512298431</v>
+        <v>55601.039010446118</v>
       </c>
       <c r="L99">
         <f t="shared" si="3"/>
-        <v>55.587491512298435</v>
+        <v>55.601039010446122</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
@@ -14009,11 +14012,11 @@
       </c>
       <c r="K100">
         <f t="shared" si="2"/>
-        <v>44216.27807617181</v>
+        <v>43686.636287133799</v>
       </c>
       <c r="L100">
         <f t="shared" si="3"/>
-        <v>44.216278076171811</v>
+        <v>43.686636287133801</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
@@ -14049,11 +14052,11 @@
       </c>
       <c r="K101">
         <f t="shared" si="2"/>
-        <v>42550.680875778125</v>
+        <v>42219.190198342912</v>
       </c>
       <c r="L101">
         <f t="shared" si="3"/>
-        <v>42.550680875778127</v>
+        <v>42.219190198342915</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
@@ -14089,11 +14092,11 @@
       </c>
       <c r="K102">
         <f t="shared" si="2"/>
-        <v>42292.09852218625</v>
+        <v>43037.594872872942</v>
       </c>
       <c r="L102">
         <f t="shared" si="3"/>
-        <v>42.292098522186251</v>
+        <v>43.037594872872944</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
@@ -14129,11 +14132,20 @@
       </c>
       <c r="K103">
         <f t="shared" si="2"/>
-        <v>47203.23729515067</v>
+        <v>47125.144082467654</v>
       </c>
       <c r="L103">
         <f t="shared" si="3"/>
-        <v>47.203237295150672</v>
+        <v>47.125144082467656</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D105" t="s">
+        <v>31</v>
+      </c>
+      <c r="E105">
+        <f>AVERAGE(E2:E103,'500_trees'!E2:E103,'1600_trees'!E2:E103)</f>
+        <v>32303.568440835588</v>
       </c>
     </row>
   </sheetData>
@@ -14167,10 +14179,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E03253E-0D39-4936-AAA4-0033724B6785}">
-  <dimension ref="A1:L103"/>
+  <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView topLeftCell="B94" workbookViewId="0">
+      <selection activeCell="K78" sqref="K78:K79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14248,12 +14260,12 @@
         <v>230548.271656036</v>
       </c>
       <c r="K2">
-        <f>SUM(E2,G2,H2)</f>
-        <v>251352.80799865659</v>
+        <f>SUM($E$105,G2,H2)</f>
+        <v>251215.6709016962</v>
       </c>
       <c r="L2">
         <f>PRODUCT(K2,0.001)</f>
-        <v>251.3528079986566</v>
+        <v>251.2156709016962</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -14288,12 +14300,12 @@
         <v>65590.7533168792</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K80" si="0">SUM(E3,G3,H3)</f>
-        <v>90491.133451461588</v>
+        <f t="shared" ref="K3:K66" si="0">SUM($E$105,G3,H3)</f>
+        <v>91006.47934095138</v>
       </c>
       <c r="L3">
         <f t="shared" ref="L3:L80" si="1">PRODUCT(K3,0.001)</f>
-        <v>90.491133451461593</v>
+        <v>91.006479340951387</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -14329,11 +14341,11 @@
       </c>
       <c r="K4">
         <f t="shared" si="0"/>
-        <v>88258.592605590704</v>
+        <v>87878.132897775198</v>
       </c>
       <c r="L4">
         <f t="shared" si="1"/>
-        <v>88.258592605590707</v>
+        <v>87.878132897775203</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -14369,11 +14381,11 @@
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>87255.288362502892</v>
+        <v>86640.738088052298</v>
       </c>
       <c r="L5">
         <f t="shared" si="1"/>
-        <v>87.255288362502895</v>
+        <v>86.640738088052302</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -14419,11 +14431,11 @@
       </c>
       <c r="K8">
         <f t="shared" si="0"/>
-        <v>184706.061124801</v>
+        <v>184029.5542062922</v>
       </c>
       <c r="L8">
         <f t="shared" si="1"/>
-        <v>184.70606112480101</v>
+        <v>184.0295542062922</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -14459,11 +14471,11 @@
       </c>
       <c r="K9">
         <f t="shared" si="0"/>
-        <v>76817.608594894307</v>
+        <v>76080.558616082693</v>
       </c>
       <c r="L9">
         <f t="shared" si="1"/>
-        <v>76.81760859489431</v>
+        <v>76.080558616082698</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -14499,11 +14511,11 @@
       </c>
       <c r="K10">
         <f t="shared" si="0"/>
-        <v>71861.438035964806</v>
+        <v>71659.197884957786</v>
       </c>
       <c r="L10">
         <f t="shared" si="1"/>
-        <v>71.86143803596481</v>
+        <v>71.659197884957791</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -14554,11 +14566,11 @@
       </c>
       <c r="K14">
         <f t="shared" si="0"/>
-        <v>205335.65807342468</v>
+        <v>204732.7051939173</v>
       </c>
       <c r="L14">
         <f t="shared" si="1"/>
-        <v>205.3356580734247</v>
+        <v>204.7327051939173</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -14594,11 +14606,11 @@
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>158369.65847015288</v>
+        <v>158100.57814733189</v>
       </c>
       <c r="L15">
         <f t="shared" si="1"/>
-        <v>158.36965847015287</v>
+        <v>158.1005781473319</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -14634,11 +14646,11 @@
       </c>
       <c r="K16">
         <f t="shared" si="0"/>
-        <v>145627.87938117969</v>
+        <v>145150.57356969599</v>
       </c>
       <c r="L16">
         <f t="shared" si="1"/>
-        <v>145.6278793811797</v>
+        <v>145.15057356969598</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -14674,11 +14686,11 @@
       </c>
       <c r="K17">
         <f t="shared" si="0"/>
-        <v>143305.34243583589</v>
+        <v>144086.59012929609</v>
       </c>
       <c r="L17">
         <f t="shared" si="1"/>
-        <v>143.30534243583588</v>
+        <v>144.0865901292961</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -14714,11 +14726,11 @@
       </c>
       <c r="K18">
         <f t="shared" si="0"/>
-        <v>152647.95589446981</v>
+        <v>152656.82752744411</v>
       </c>
       <c r="L18">
         <f t="shared" si="1"/>
-        <v>152.64795589446982</v>
+        <v>152.65682752744411</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -14754,11 +14766,11 @@
       </c>
       <c r="K19">
         <f t="shared" si="0"/>
-        <v>150387.13645935021</v>
+        <v>150685.4444326566</v>
       </c>
       <c r="L19">
         <f t="shared" si="1"/>
-        <v>150.38713645935022</v>
+        <v>150.6854444326566</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -14794,11 +14806,11 @@
       </c>
       <c r="K20">
         <f t="shared" si="0"/>
-        <v>119518.52321624741</v>
+        <v>119565.2306856322</v>
       </c>
       <c r="L20">
         <f t="shared" si="1"/>
-        <v>119.51852321624742</v>
+        <v>119.5652306856322</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -14834,11 +14846,11 @@
       </c>
       <c r="K21">
         <f t="shared" si="0"/>
-        <v>57455.948114394996</v>
+        <v>57382.726985375884</v>
       </c>
       <c r="L21">
         <f t="shared" si="1"/>
-        <v>57.455948114394999</v>
+        <v>57.382726985375882</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -14874,11 +14886,11 @@
       </c>
       <c r="K22">
         <f t="shared" si="0"/>
-        <v>53451.896667480418</v>
+        <v>53154.49174062501</v>
       </c>
       <c r="L22">
         <f t="shared" si="1"/>
-        <v>53.451896667480419</v>
+        <v>53.154491740625012</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -14914,11 +14926,11 @@
       </c>
       <c r="K23">
         <f t="shared" si="0"/>
-        <v>53984.684705734151</v>
+        <v>53568.959552209439</v>
       </c>
       <c r="L23">
         <f t="shared" si="1"/>
-        <v>53.984684705734153</v>
+        <v>53.568959552209442</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -14954,11 +14966,11 @@
       </c>
       <c r="K24">
         <f t="shared" si="0"/>
-        <v>54624.42111968981</v>
+        <v>53763.059932153294</v>
       </c>
       <c r="L24">
         <f t="shared" si="1"/>
-        <v>54.624421119689814</v>
+        <v>53.763059932153297</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -14999,11 +15011,11 @@
       </c>
       <c r="K26">
         <f t="shared" si="0"/>
-        <v>161607.08069801243</v>
+        <v>161702.15852872544</v>
       </c>
       <c r="L26">
         <f t="shared" si="1"/>
-        <v>161.60708069801242</v>
+        <v>161.70215852872545</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -15039,11 +15051,11 @@
       </c>
       <c r="K27">
         <f t="shared" si="0"/>
-        <v>61105.694770812894</v>
+        <v>61743.677216928081</v>
       </c>
       <c r="L27">
         <f t="shared" si="1"/>
-        <v>61.105694770812896</v>
+        <v>61.743677216928084</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -15079,11 +15091,11 @@
       </c>
       <c r="K28">
         <f t="shared" si="0"/>
-        <v>45118.538618087667</v>
+        <v>45583.540994088762</v>
       </c>
       <c r="L28">
         <f t="shared" si="1"/>
-        <v>45.118538618087669</v>
+        <v>45.583540994088764</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
@@ -15119,11 +15131,11 @@
       </c>
       <c r="K29">
         <f t="shared" si="0"/>
-        <v>45789.994716644185</v>
+        <v>45215.932208459475</v>
       </c>
       <c r="L29">
         <f t="shared" si="1"/>
-        <v>45.789994716644188</v>
+        <v>45.215932208459478</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -15159,11 +15171,11 @@
       </c>
       <c r="K30">
         <f t="shared" si="0"/>
-        <v>46439.265012741031</v>
+        <v>45982.697564523318</v>
       </c>
       <c r="L30">
         <f t="shared" si="1"/>
-        <v>46.439265012741032</v>
+        <v>45.98269756452332</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -15199,11 +15211,11 @@
       </c>
       <c r="K31">
         <f t="shared" si="0"/>
-        <v>48275.81071853629</v>
+        <v>47606.086093347178</v>
       </c>
       <c r="L31">
         <f t="shared" si="1"/>
-        <v>48.275810718536292</v>
+        <v>47.60608609334718</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -15239,11 +15251,11 @@
       </c>
       <c r="K32">
         <f t="shared" si="0"/>
-        <v>268142.75312423677</v>
+        <v>267977.77779714338</v>
       </c>
       <c r="L32">
         <f t="shared" si="1"/>
-        <v>268.14275312423678</v>
+        <v>267.9777777971434</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -15279,11 +15291,11 @@
       </c>
       <c r="K33">
         <f t="shared" si="0"/>
-        <v>91547.536611556905</v>
+        <v>91054.701644341985</v>
       </c>
       <c r="L33">
         <f t="shared" si="1"/>
-        <v>91.547536611556907</v>
+        <v>91.054701644341989</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -15319,11 +15331,11 @@
       </c>
       <c r="K34">
         <f t="shared" si="0"/>
-        <v>87401.150465011408</v>
+        <v>87301.957923333583</v>
       </c>
       <c r="L34">
         <f t="shared" si="1"/>
-        <v>87.401150465011412</v>
+        <v>87.301957923333589</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -15359,11 +15371,11 @@
       </c>
       <c r="K35">
         <f t="shared" si="0"/>
-        <v>85755.883693694894</v>
+        <v>86128.751832406473</v>
       </c>
       <c r="L35">
         <f t="shared" si="1"/>
-        <v>85.755883693694898</v>
+        <v>86.128751832406479</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -15409,11 +15421,11 @@
       </c>
       <c r="K38">
         <f t="shared" si="0"/>
-        <v>188180.339336395</v>
+        <v>188139.492589395</v>
       </c>
       <c r="L38">
         <f t="shared" si="1"/>
-        <v>188.18033933639501</v>
+        <v>188.13949258939499</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -15449,11 +15461,11 @@
       </c>
       <c r="K39">
         <f t="shared" si="0"/>
-        <v>76728.801488876197</v>
+        <v>76344.123441140691</v>
       </c>
       <c r="L39">
         <f t="shared" si="1"/>
-        <v>76.728801488876201</v>
+        <v>76.344123441140695</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -15489,11 +15501,11 @@
       </c>
       <c r="K40">
         <f t="shared" si="0"/>
-        <v>72449.626445770104</v>
+        <v>71787.981826226693</v>
       </c>
       <c r="L40">
         <f t="shared" si="1"/>
-        <v>72.449626445770107</v>
+        <v>71.787981826226698</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
@@ -15544,11 +15556,11 @@
       </c>
       <c r="K44">
         <f t="shared" si="0"/>
-        <v>185247.31183051979</v>
+        <v>185889.06438962626</v>
       </c>
       <c r="L44">
         <f t="shared" si="1"/>
-        <v>185.24731183051978</v>
+        <v>185.88906438962627</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
@@ -15584,11 +15596,11 @@
       </c>
       <c r="K45">
         <f t="shared" si="0"/>
-        <v>155706.45451545651</v>
+        <v>155796.10736982059</v>
       </c>
       <c r="L45">
         <f t="shared" si="1"/>
-        <v>155.70645451545653</v>
+        <v>155.79610736982059</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -15624,11 +15636,11 @@
       </c>
       <c r="K46">
         <f t="shared" si="0"/>
-        <v>145073.46439361482</v>
+        <v>145395.86146489781</v>
       </c>
       <c r="L46">
         <f t="shared" si="1"/>
-        <v>145.07346439361481</v>
+        <v>145.39586146489782</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -15664,11 +15676,11 @@
       </c>
       <c r="K47">
         <f t="shared" si="0"/>
-        <v>140366.62077903739</v>
+        <v>140899.97943059687</v>
       </c>
       <c r="L47">
         <f t="shared" si="1"/>
-        <v>140.36662077903739</v>
+        <v>140.89997943059686</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
@@ -15704,11 +15716,11 @@
       </c>
       <c r="K48">
         <f t="shared" si="0"/>
-        <v>144989.853858947</v>
+        <v>145536.90989629447</v>
       </c>
       <c r="L48">
         <f t="shared" si="1"/>
-        <v>144.98985385894699</v>
+        <v>145.53690989629447</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
@@ -15744,11 +15756,11 @@
       </c>
       <c r="K49">
         <f t="shared" si="0"/>
-        <v>145794.8923110961</v>
+        <v>146214.33885709528</v>
       </c>
       <c r="L49">
         <f t="shared" si="1"/>
-        <v>145.79489231109611</v>
+        <v>146.21433885709527</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
@@ -15784,11 +15796,11 @@
       </c>
       <c r="K50">
         <f t="shared" si="0"/>
-        <v>119909.574985504</v>
+        <v>120686.21047155139</v>
       </c>
       <c r="L50">
         <f t="shared" si="1"/>
-        <v>119.90957498550401</v>
+        <v>120.68621047155139</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
@@ -15824,11 +15836,11 @@
       </c>
       <c r="K51">
         <f t="shared" si="0"/>
-        <v>56518.7549591063</v>
+        <v>57018.347579400586</v>
       </c>
       <c r="L51">
         <f t="shared" si="1"/>
-        <v>56.518754959106303</v>
+        <v>57.01834757940059</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -15864,11 +15876,11 @@
       </c>
       <c r="K52">
         <f t="shared" si="0"/>
-        <v>52944.219827651905</v>
+        <v>52967.95995847469</v>
       </c>
       <c r="L52">
         <f t="shared" si="1"/>
-        <v>52.944219827651906</v>
+        <v>52.967959958474694</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -15904,11 +15916,11 @@
       </c>
       <c r="K53">
         <f t="shared" si="0"/>
-        <v>53384.316682815523</v>
+        <v>53098.176318566912</v>
       </c>
       <c r="L53">
         <f t="shared" si="1"/>
-        <v>53.384316682815523</v>
+        <v>53.098176318566914</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -15944,11 +15956,11 @@
       </c>
       <c r="K54">
         <f t="shared" si="0"/>
-        <v>52779.498338699254</v>
+        <v>52620.731192987034</v>
       </c>
       <c r="L54">
         <f t="shared" si="1"/>
-        <v>52.779498338699256</v>
+        <v>52.620731192987037</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.3">
@@ -15989,11 +16001,11 @@
       </c>
       <c r="K56">
         <f t="shared" si="0"/>
-        <v>157076.0350227353</v>
+        <v>156672.5498022245</v>
       </c>
       <c r="L56">
         <f t="shared" si="1"/>
-        <v>157.07603502273531</v>
+        <v>156.67254980222449</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
@@ -16029,11 +16041,11 @@
       </c>
       <c r="K57">
         <f t="shared" si="0"/>
-        <v>61904.497861862081</v>
+        <v>61875.750857751467</v>
       </c>
       <c r="L57">
         <f t="shared" si="1"/>
-        <v>61.904497861862083</v>
+        <v>61.87575085775147</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
@@ -16069,11 +16081,11 @@
       </c>
       <c r="K58">
         <f t="shared" si="0"/>
-        <v>44429.619550704905</v>
+        <v>44087.995606820688</v>
       </c>
       <c r="L58">
         <f t="shared" si="1"/>
-        <v>44.429619550704906</v>
+        <v>44.087995606820691</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -16109,11 +16121,11 @@
       </c>
       <c r="K59">
         <f t="shared" si="0"/>
-        <v>44365.172147750767</v>
+        <v>43538.127499978655</v>
       </c>
       <c r="L59">
         <f t="shared" si="1"/>
-        <v>44.365172147750769</v>
+        <v>43.538127499978657</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
@@ -16149,11 +16161,11 @@
       </c>
       <c r="K60">
         <f t="shared" si="0"/>
-        <v>43132.436513900677</v>
+        <v>43034.369307916269</v>
       </c>
       <c r="L60">
         <f t="shared" si="1"/>
-        <v>43.132436513900679</v>
+        <v>43.034369307916272</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
@@ -16189,11 +16201,11 @@
       </c>
       <c r="K61">
         <f t="shared" si="0"/>
-        <v>43240.35453796378</v>
+        <v>43598.816710870371</v>
       </c>
       <c r="L61">
         <f t="shared" si="1"/>
-        <v>43.240354537963782</v>
+        <v>43.598816710870373</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
@@ -16229,11 +16241,11 @@
       </c>
       <c r="K62">
         <f t="shared" si="0"/>
-        <v>2685956.4723968492</v>
+        <v>2685678.8712324295</v>
       </c>
       <c r="L62">
         <f t="shared" si="1"/>
-        <v>2685.9564723968492</v>
+        <v>2685.6788712324296</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.3">
@@ -16269,11 +16281,11 @@
       </c>
       <c r="K63">
         <f t="shared" si="0"/>
-        <v>316206.54249191203</v>
+        <v>316019.73660604173</v>
       </c>
       <c r="L63">
         <f t="shared" si="1"/>
-        <v>316.20654249191205</v>
+        <v>316.01973660604176</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.3">
@@ -16309,11 +16321,11 @@
       </c>
       <c r="K64">
         <f t="shared" si="0"/>
-        <v>77251.113414764302</v>
+        <v>77129.876452844182</v>
       </c>
       <c r="L64">
         <f t="shared" si="1"/>
-        <v>77.251113414764305</v>
+        <v>77.129876452844186</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.3">
@@ -16349,11 +16361,11 @@
       </c>
       <c r="K65">
         <f t="shared" si="0"/>
-        <v>56933.135509490807</v>
+        <v>56565.353232781883</v>
       </c>
       <c r="L65">
         <f t="shared" si="1"/>
-        <v>56.93313550949081</v>
+        <v>56.565353232781881</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
@@ -16389,11 +16401,11 @@
       </c>
       <c r="K66">
         <f t="shared" si="0"/>
-        <v>55709.134578704601</v>
+        <v>55465.203601281588</v>
       </c>
       <c r="L66">
         <f t="shared" si="1"/>
-        <v>55.7091345787046</v>
+        <v>55.465203601281587</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.3">
@@ -16428,12 +16440,12 @@
         <v>22916.711091995199</v>
       </c>
       <c r="K67">
-        <f t="shared" si="0"/>
-        <v>56498.334646224903</v>
+        <f t="shared" ref="K67:K103" si="2">SUM($E$105,G67,H67)</f>
+        <v>55218.277293603489</v>
       </c>
       <c r="L67">
         <f t="shared" si="1"/>
-        <v>56.498334646224905</v>
+        <v>55.218277293603492</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
@@ -16468,12 +16480,12 @@
         <v>2709290.5011176998</v>
       </c>
       <c r="K68">
-        <f t="shared" si="0"/>
-        <v>2742188.3225440886</v>
+        <f t="shared" si="2"/>
+        <v>2741592.0580209806</v>
       </c>
       <c r="L68">
         <f t="shared" si="1"/>
-        <v>2742.1883225440888</v>
+        <v>2741.5920580209804</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
@@ -16508,12 +16520,12 @@
         <v>282682.777166366</v>
       </c>
       <c r="K69">
-        <f t="shared" si="0"/>
-        <v>315026.81159973057</v>
+        <f t="shared" si="2"/>
+        <v>314984.42943708104</v>
       </c>
       <c r="L69">
         <f t="shared" si="1"/>
-        <v>315.02681159973059</v>
+        <v>314.98442943708102</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
@@ -16548,12 +16560,12 @@
         <v>43091.085195541302</v>
       </c>
       <c r="K70">
-        <f t="shared" si="0"/>
-        <v>74526.298999786202</v>
+        <f t="shared" si="2"/>
+        <v>75392.702418725486</v>
       </c>
       <c r="L70">
         <f t="shared" si="1"/>
-        <v>74.526298999786206</v>
+        <v>75.392702418725491</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
@@ -16588,12 +16600,12 @@
         <v>21385.6880664825</v>
       </c>
       <c r="K71">
-        <f t="shared" si="0"/>
-        <v>53278.7222862243</v>
+        <f t="shared" si="2"/>
+        <v>53687.308865945393</v>
       </c>
       <c r="L71">
         <f t="shared" si="1"/>
-        <v>53.278722286224301</v>
+        <v>53.687308865945397</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
@@ -16628,12 +16640,12 @@
         <v>21289.058685302702</v>
       </c>
       <c r="K72">
-        <f t="shared" si="0"/>
-        <v>53645.679712295459</v>
+        <f t="shared" si="2"/>
+        <v>53590.669948022449</v>
       </c>
       <c r="L72">
         <f t="shared" si="1"/>
-        <v>53.645679712295461</v>
+        <v>53.590669948022452</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
@@ -16668,12 +16680,12 @@
         <v>20943.4785842895</v>
       </c>
       <c r="K73">
-        <f t="shared" si="0"/>
-        <v>53417.61469840991</v>
+        <f t="shared" si="2"/>
+        <v>53245.069819848599</v>
       </c>
       <c r="L73">
         <f t="shared" si="1"/>
-        <v>53.417614698409913</v>
+        <v>53.245069819848602</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
@@ -16708,12 +16720,12 @@
         <v>254850.12674331601</v>
       </c>
       <c r="K74">
-        <f t="shared" si="0"/>
-        <v>276279.92200851411</v>
+        <f t="shared" si="2"/>
+        <v>276147.67654554121</v>
       </c>
       <c r="L74">
         <f t="shared" si="1"/>
-        <v>276.27992200851412</v>
+        <v>276.14767654554123</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
@@ -16748,12 +16760,12 @@
         <v>70100.028276443394</v>
       </c>
       <c r="K75">
-        <f t="shared" si="0"/>
-        <v>91676.445722579796</v>
+        <f t="shared" si="2"/>
+        <v>91345.20252362969</v>
       </c>
       <c r="L75">
         <f t="shared" si="1"/>
-        <v>91.6764457225798</v>
+        <v>91.345202523629695</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
@@ -16788,12 +16800,12 @@
         <v>65597.169160842896</v>
       </c>
       <c r="K76">
-        <f t="shared" si="0"/>
-        <v>87616.528034210103</v>
+        <f t="shared" si="2"/>
+        <v>86800.769168298284</v>
       </c>
       <c r="L76">
         <f t="shared" si="1"/>
-        <v>87.616528034210106</v>
+        <v>86.800769168298288</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
@@ -16828,12 +16840,12 @@
         <v>65286.664962768496</v>
       </c>
       <c r="K77">
-        <f t="shared" si="0"/>
-        <v>85861.827135085899</v>
+        <f t="shared" si="2"/>
+        <v>86201.553183953787</v>
       </c>
       <c r="L77">
         <f t="shared" si="1"/>
-        <v>85.861827135085903</v>
+        <v>86.201553183953791</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
@@ -16878,12 +16890,12 @@
         <v>167694.749116897</v>
       </c>
       <c r="K80">
-        <f t="shared" si="0"/>
-        <v>189892.6761150352</v>
+        <f t="shared" si="2"/>
+        <v>189089.70149175337</v>
       </c>
       <c r="L80">
         <f t="shared" si="1"/>
-        <v>189.89267611503519</v>
+        <v>189.08970149175337</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
@@ -16918,12 +16930,12 @@
         <v>55217.929601669297</v>
       </c>
       <c r="K81">
-        <f t="shared" ref="K81:K103" si="2">SUM(E81,G81,H81)</f>
-        <v>76688.775300979396</v>
+        <f t="shared" si="2"/>
+        <v>76556.335765283089</v>
       </c>
       <c r="L81">
         <f t="shared" ref="L81:L103" si="3">PRODUCT(K81,0.001)</f>
-        <v>76.688775300979401</v>
+        <v>76.556335765283094</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
@@ -16959,11 +16971,11 @@
       </c>
       <c r="K82">
         <f t="shared" si="2"/>
-        <v>73087.726354598795</v>
+        <v>72195.126372735482</v>
       </c>
       <c r="L82">
         <f t="shared" si="3"/>
-        <v>73.0877263545988</v>
+        <v>72.195126372735487</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
@@ -17014,11 +17026,11 @@
       </c>
       <c r="K86">
         <f t="shared" si="2"/>
-        <v>206247.6415634146</v>
+        <v>206431.75061361</v>
       </c>
       <c r="L86">
         <f t="shared" si="3"/>
-        <v>206.24764156341459</v>
+        <v>206.43175061361001</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
@@ -17054,11 +17066,11 @@
       </c>
       <c r="K87">
         <f t="shared" si="2"/>
-        <v>157993.14141273388</v>
+        <v>158291.33184568078</v>
       </c>
       <c r="L87">
         <f t="shared" si="3"/>
-        <v>157.99314141273388</v>
+        <v>158.29133184568079</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
@@ -17094,11 +17106,11 @@
       </c>
       <c r="K88">
         <f t="shared" si="2"/>
-        <v>146691.92647933931</v>
+        <v>147100.50948278178</v>
       </c>
       <c r="L88">
         <f t="shared" si="3"/>
-        <v>146.69192647933932</v>
+        <v>147.10050948278177</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
@@ -17134,11 +17146,11 @@
       </c>
       <c r="K89">
         <f t="shared" si="2"/>
-        <v>146746.67930602969</v>
+        <v>146543.41347829541</v>
       </c>
       <c r="L89">
         <f t="shared" si="3"/>
-        <v>146.74667930602971</v>
+        <v>146.54341347829541</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
@@ -17174,11 +17186,11 @@
       </c>
       <c r="K90">
         <f t="shared" si="2"/>
-        <v>149702.20589637652</v>
+        <v>150120.23027555141</v>
       </c>
       <c r="L90">
         <f t="shared" si="3"/>
-        <v>149.70220589637651</v>
+        <v>150.12023027555142</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
@@ -17214,11 +17226,11 @@
       </c>
       <c r="K91">
         <f t="shared" si="2"/>
-        <v>151815.9487247458</v>
+        <v>152266.73181668919</v>
       </c>
       <c r="L91">
         <f t="shared" si="3"/>
-        <v>151.81594872474579</v>
+        <v>152.2667318166892</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
@@ -17254,11 +17266,11 @@
       </c>
       <c r="K92">
         <f t="shared" si="2"/>
-        <v>120978.07788848859</v>
+        <v>121372.8133024383</v>
       </c>
       <c r="L92">
         <f t="shared" si="3"/>
-        <v>120.9780778884886</v>
+        <v>121.3728133024383</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
@@ -17294,11 +17306,11 @@
       </c>
       <c r="K93">
         <f t="shared" si="2"/>
-        <v>57039.595842361297</v>
+        <v>57437.844592492591</v>
       </c>
       <c r="L93">
         <f t="shared" si="3"/>
-        <v>57.039595842361301</v>
+        <v>57.437844592492596</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
@@ -17334,11 +17346,11 @@
       </c>
       <c r="K94">
         <f t="shared" si="2"/>
-        <v>53397.627353668046</v>
+        <v>52791.416961114432</v>
       </c>
       <c r="L94">
         <f t="shared" si="3"/>
-        <v>53.397627353668049</v>
+        <v>52.791416961114436</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
@@ -17374,11 +17386,11 @@
       </c>
       <c r="K95">
         <f t="shared" si="2"/>
-        <v>53220.368623733448</v>
+        <v>52516.989308755437</v>
       </c>
       <c r="L95">
         <f t="shared" si="3"/>
-        <v>53.220368623733449</v>
+        <v>52.516989308755441</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
@@ -17414,11 +17426,11 @@
       </c>
       <c r="K96">
         <f t="shared" si="2"/>
-        <v>53407.183885574254</v>
+        <v>52792.497235696341</v>
       </c>
       <c r="L96">
         <f t="shared" si="3"/>
-        <v>53.407183885574256</v>
+        <v>52.792497235696345</v>
       </c>
     </row>
     <row r="97" spans="1:12" x14ac:dyDescent="0.3">
@@ -17459,11 +17471,11 @@
       </c>
       <c r="K98">
         <f t="shared" si="2"/>
-        <v>162036.64135932917</v>
+        <v>161922.89646283875</v>
       </c>
       <c r="L98">
         <f t="shared" si="3"/>
-        <v>162.03664135932917</v>
+        <v>161.92289646283876</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
@@ -17499,11 +17511,11 @@
       </c>
       <c r="K99">
         <f t="shared" si="2"/>
-        <v>60320.321798324498</v>
+        <v>59705.051022927786</v>
       </c>
       <c r="L99">
         <f t="shared" si="3"/>
-        <v>60.3203217983245</v>
+        <v>59.70505102292779</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
@@ -17539,11 +17551,11 @@
       </c>
       <c r="K100">
         <f t="shared" si="2"/>
-        <v>46380.381107330308</v>
+        <v>45913.894730966196</v>
       </c>
       <c r="L100">
         <f t="shared" si="3"/>
-        <v>46.380381107330308</v>
+        <v>45.913894730966199</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
@@ -17579,11 +17591,11 @@
       </c>
       <c r="K101">
         <f t="shared" si="2"/>
-        <v>45928.158044815013</v>
+        <v>45447.910148065203</v>
       </c>
       <c r="L101">
         <f t="shared" si="3"/>
-        <v>45.928158044815014</v>
+        <v>45.447910148065205</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
@@ -17619,11 +17631,11 @@
       </c>
       <c r="K102">
         <f t="shared" si="2"/>
-        <v>46315.216779708797</v>
+        <v>46053.336697976687</v>
       </c>
       <c r="L102">
         <f t="shared" si="3"/>
-        <v>46.315216779708798</v>
+        <v>46.05333669797669</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
@@ -17659,11 +17671,20 @@
       </c>
       <c r="K103">
         <f t="shared" si="2"/>
-        <v>48093.544960021878</v>
+        <v>47476.194220941165</v>
       </c>
       <c r="L103">
         <f t="shared" si="3"/>
-        <v>48.09354496002188</v>
+        <v>47.476194220941167</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D105" t="s">
+        <v>31</v>
+      </c>
+      <c r="E105">
+        <f>'10_trees'!E105</f>
+        <v>32303.568440835588</v>
       </c>
     </row>
   </sheetData>
@@ -17697,10 +17718,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F05BF744-05C7-436C-91E4-82408DA3D1D3}">
-  <dimension ref="A1:L103"/>
+  <dimension ref="A1:L105"/>
   <sheetViews>
-    <sheetView topLeftCell="A84" workbookViewId="0">
-      <selection activeCell="D73" sqref="D73"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="K96" sqref="K96:K97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17778,12 +17799,12 @@
         <v>239546.39720916699</v>
       </c>
       <c r="K2">
-        <f>SUM(E2,G2,H2)</f>
-        <v>254482.07664489732</v>
+        <f>SUM($E$105,G2,H2)</f>
+        <v>254191.23037473441</v>
       </c>
       <c r="L2">
         <f>PRODUCT(K2,0.001)</f>
-        <v>254.48207664489732</v>
+        <v>254.19123037473443</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
@@ -17818,12 +17839,12 @@
         <v>165036.49902343701</v>
       </c>
       <c r="K3">
-        <f>SUM(E3,G3,H3)</f>
-        <v>184997.14636802592</v>
+        <f t="shared" ref="K3:K66" si="0">SUM($E$105,G3,H3)</f>
+        <v>184905.68574086839</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L91" si="0">PRODUCT(K3,0.001)</f>
-        <v>184.99714636802591</v>
+        <f t="shared" ref="L3:L91" si="1">PRODUCT(K3,0.001)</f>
+        <v>184.90568574086839</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
@@ -17858,12 +17879,12 @@
         <v>158555.198192596</v>
       </c>
       <c r="K4">
-        <f t="shared" ref="K4:K92" si="1">SUM(E4,G4,H4)</f>
-        <v>178330.80959320031</v>
+        <f t="shared" si="0"/>
+        <v>178324.5092214749</v>
       </c>
       <c r="L4">
-        <f t="shared" si="0"/>
-        <v>178.33080959320031</v>
+        <f t="shared" si="1"/>
+        <v>178.3245092214749</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -17898,12 +17919,12 @@
         <v>158808.76493453901</v>
       </c>
       <c r="K5">
+        <f t="shared" si="0"/>
+        <v>178583.04222242086</v>
+      </c>
+      <c r="L5">
         <f t="shared" si="1"/>
-        <v>178713.28425407369</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="0"/>
-        <v>178.7132842540737</v>
+        <v>178.58304222242086</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.3">
@@ -17948,12 +17969,12 @@
         <v>162770.67875862101</v>
       </c>
       <c r="K8">
+        <f t="shared" si="0"/>
+        <v>183093.8959898155</v>
+      </c>
+      <c r="L8">
         <f t="shared" si="1"/>
-        <v>183815.19865989601</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="0"/>
-        <v>183.815198659896</v>
+        <v>183.09389598981551</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
@@ -17988,12 +18009,12 @@
         <v>112366.970062255</v>
       </c>
       <c r="K9">
+        <f t="shared" si="0"/>
+        <v>133076.7250837493</v>
+      </c>
+      <c r="L9">
         <f t="shared" si="1"/>
-        <v>132436.5928173064</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="0"/>
-        <v>132.4365928173064</v>
+        <v>133.0767250837493</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
@@ -18028,12 +18049,12 @@
         <v>106663.91015052699</v>
       </c>
       <c r="K10">
+        <f t="shared" si="0"/>
+        <v>127199.57955495598</v>
+      </c>
+      <c r="L10">
         <f t="shared" si="1"/>
-        <v>127318.0851936339</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="0"/>
-        <v>127.31808519363391</v>
+        <v>127.19957955495599</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.3">
@@ -18083,12 +18104,12 @@
         <v>578580.73878288199</v>
       </c>
       <c r="K14">
+        <f t="shared" si="0"/>
+        <v>580269.542056481</v>
+      </c>
+      <c r="L14">
         <f t="shared" si="1"/>
-        <v>580944.63896751299</v>
-      </c>
-      <c r="L14">
-        <f t="shared" si="0"/>
-        <v>580.94463896751301</v>
+        <v>580.26954205648099</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -18123,12 +18144,12 @@
         <v>392787.50658035203</v>
       </c>
       <c r="K15">
+        <f t="shared" si="0"/>
+        <v>401936.7726625608</v>
+      </c>
+      <c r="L15">
         <f t="shared" si="1"/>
-        <v>401977.77056694002</v>
-      </c>
-      <c r="L15">
-        <f t="shared" si="0"/>
-        <v>401.97777056694002</v>
+        <v>401.93677266256083</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -18163,12 +18184,12 @@
         <v>343485.116720199</v>
       </c>
       <c r="K16">
+        <f t="shared" si="0"/>
+        <v>354053.47927228658</v>
+      </c>
+      <c r="L16">
         <f t="shared" si="1"/>
-        <v>354057.26432800252</v>
-      </c>
-      <c r="L16">
-        <f t="shared" si="0"/>
-        <v>354.05726432800253</v>
+        <v>354.05347927228661</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -18203,12 +18224,12 @@
         <v>345331.50982856698</v>
       </c>
       <c r="K17">
+        <f t="shared" si="0"/>
+        <v>350833.67522374826</v>
+      </c>
+      <c r="L17">
         <f t="shared" si="1"/>
-        <v>350423.66218566836</v>
-      </c>
-      <c r="L17">
-        <f t="shared" si="0"/>
-        <v>350.42366218566838</v>
+        <v>350.83367522374829</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -18243,12 +18264,12 @@
         <v>354891.96133613499</v>
       </c>
       <c r="K18">
+        <f t="shared" si="0"/>
+        <v>364859.65259687102</v>
+      </c>
+      <c r="L18">
         <f t="shared" si="1"/>
-        <v>365147.02486991783</v>
-      </c>
-      <c r="L18">
-        <f t="shared" si="0"/>
-        <v>365.14702486991786</v>
+        <v>364.859652596871</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -18283,12 +18304,12 @@
         <v>347964.46394920303</v>
       </c>
       <c r="K19">
+        <f t="shared" si="0"/>
+        <v>357027.28350774455</v>
+      </c>
+      <c r="L19">
         <f t="shared" si="1"/>
-        <v>356396.47436141875</v>
-      </c>
-      <c r="L19">
-        <f t="shared" si="0"/>
-        <v>356.39647436141877</v>
+        <v>357.02728350774453</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -18323,12 +18344,12 @@
         <v>133443.95208358701</v>
       </c>
       <c r="K20">
+        <f t="shared" si="0"/>
+        <v>130869.30258886109</v>
+      </c>
+      <c r="L20">
         <f t="shared" si="1"/>
-        <v>131053.35164070121</v>
-      </c>
-      <c r="L20">
-        <f t="shared" si="0"/>
-        <v>131.05335164070121</v>
+        <v>130.8693025888611</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -18363,12 +18384,12 @@
         <v>86816.240549087495</v>
       </c>
       <c r="K21">
+        <f t="shared" si="0"/>
+        <v>75610.659200112801</v>
+      </c>
+      <c r="L21">
         <f t="shared" si="1"/>
-        <v>76128.954887389904</v>
-      </c>
-      <c r="L21">
-        <f t="shared" si="0"/>
-        <v>76.128954887389909</v>
+        <v>75.610659200112806</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -18403,12 +18424,12 @@
         <v>95505.797147750796</v>
       </c>
       <c r="K22">
+        <f t="shared" si="0"/>
+        <v>72399.943190972786</v>
+      </c>
+      <c r="L22">
         <f t="shared" si="1"/>
-        <v>72432.852029800197</v>
-      </c>
-      <c r="L22">
-        <f t="shared" si="0"/>
-        <v>72.432852029800202</v>
+        <v>72.399943190972792</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -18443,12 +18464,12 @@
         <v>187336.53521537699</v>
       </c>
       <c r="K23">
+        <f t="shared" si="0"/>
+        <v>72369.791346948186</v>
+      </c>
+      <c r="L23">
         <f t="shared" si="1"/>
-        <v>72764.304399490196</v>
-      </c>
-      <c r="L23">
-        <f t="shared" si="0"/>
-        <v>72.7643043994902</v>
+        <v>72.36979134694819</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -18493,12 +18514,12 @@
         <v>159535.32123565601</v>
       </c>
       <c r="K26">
+        <f t="shared" si="0"/>
+        <v>184464.74106923741</v>
+      </c>
+      <c r="L26">
         <f t="shared" si="1"/>
-        <v>184368.63374709993</v>
-      </c>
-      <c r="L26">
-        <f t="shared" si="0"/>
-        <v>184.36863374709992</v>
+        <v>184.46474106923742</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -18533,12 +18554,12 @@
         <v>34365.540981292703</v>
       </c>
       <c r="K27">
+        <f t="shared" si="0"/>
+        <v>63804.502326409907</v>
+      </c>
+      <c r="L27">
         <f t="shared" si="1"/>
-        <v>63830.584526061924</v>
-      </c>
-      <c r="L27">
-        <f t="shared" si="0"/>
-        <v>63.830584526061926</v>
+        <v>63.80450232640991</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
@@ -18573,12 +18594,12 @@
         <v>28558.894157409599</v>
       </c>
       <c r="K28">
+        <f t="shared" si="0"/>
+        <v>57993.60640661011</v>
+      </c>
+      <c r="L28">
         <f t="shared" si="1"/>
-        <v>57542.337894439625</v>
-      </c>
-      <c r="L28">
-        <f t="shared" si="0"/>
-        <v>57.542337894439626</v>
+        <v>57.993606406610112</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
@@ -18613,12 +18634,12 @@
         <v>29049.742221832199</v>
       </c>
       <c r="K29">
+        <f t="shared" si="0"/>
+        <v>58477.742034356663</v>
+      </c>
+      <c r="L29">
         <f t="shared" si="1"/>
-        <v>58666.169404983477</v>
-      </c>
-      <c r="L29">
-        <f t="shared" si="0"/>
-        <v>58.666169404983478</v>
+        <v>58.477742034356666</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
@@ -18653,12 +18674,12 @@
         <v>29913.5887622833</v>
       </c>
       <c r="K30">
+        <f t="shared" si="0"/>
+        <v>59336.269217889341</v>
+      </c>
+      <c r="L30">
         <f t="shared" si="1"/>
-        <v>60144.439935684051</v>
-      </c>
-      <c r="L30">
-        <f t="shared" si="0"/>
-        <v>60.144439935684055</v>
+        <v>59.336269217889345</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
@@ -18693,12 +18714,12 @@
         <v>31841.180801391602</v>
       </c>
       <c r="K31">
+        <f t="shared" si="0"/>
+        <v>61255.60696737055</v>
+      </c>
+      <c r="L31">
         <f t="shared" si="1"/>
-        <v>61890.54465293877</v>
-      </c>
-      <c r="L31">
-        <f t="shared" si="0"/>
-        <v>61.890544652938772</v>
+        <v>61.255606967370554</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
@@ -18733,12 +18754,12 @@
         <v>314056.14852905198</v>
       </c>
       <c r="K32">
+        <f t="shared" si="0"/>
+        <v>266155.06156102882</v>
+      </c>
+      <c r="L32">
         <f t="shared" si="1"/>
-        <v>266882.96341896022</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="0"/>
-        <v>266.88296341896023</v>
+        <v>266.15506156102884</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
@@ -18773,12 +18794,12 @@
         <v>226867.37537384001</v>
       </c>
       <c r="K33">
+        <f t="shared" si="0"/>
+        <v>181793.31668035258</v>
+      </c>
+      <c r="L33">
         <f t="shared" si="1"/>
-        <v>182120.86486816377</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="0"/>
-        <v>182.12086486816378</v>
+        <v>181.79331668035258</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.3">
@@ -18813,12 +18834,12 @@
         <v>221914.10136222799</v>
       </c>
       <c r="K34">
+        <f t="shared" si="0"/>
+        <v>176649.30804387739</v>
+      </c>
+      <c r="L34">
         <f t="shared" si="1"/>
-        <v>176606.73642158418</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="0"/>
-        <v>176.60673642158417</v>
+        <v>176.6493080438774</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.3">
@@ -18853,12 +18874,12 @@
         <v>224602.76794433501</v>
       </c>
       <c r="K35">
+        <f t="shared" si="0"/>
+        <v>177296.38798848787</v>
+      </c>
+      <c r="L35">
         <f t="shared" si="1"/>
-        <v>176637.19844818019</v>
-      </c>
-      <c r="L35">
-        <f t="shared" si="0"/>
-        <v>176.63719844818019</v>
+        <v>177.29638798848788</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
@@ -18903,12 +18924,12 @@
         <v>230593.57929229701</v>
       </c>
       <c r="K38">
+        <f t="shared" si="0"/>
+        <v>185667.18156949748</v>
+      </c>
+      <c r="L38">
         <f t="shared" si="1"/>
-        <v>185994.662761688</v>
-      </c>
-      <c r="L38">
-        <f t="shared" si="0"/>
-        <v>185.99466276168801</v>
+        <v>185.66718156949747</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
@@ -18943,12 +18964,12 @@
         <v>174856.493711471</v>
       </c>
       <c r="K39">
+        <f t="shared" si="0"/>
+        <v>130738.16879407648</v>
+      </c>
+      <c r="L39">
         <f t="shared" si="1"/>
-        <v>130909.4660282134</v>
-      </c>
-      <c r="L39">
-        <f t="shared" si="0"/>
-        <v>130.90946602821342</v>
+        <v>130.73816879407647</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
@@ -18983,12 +19004,12 @@
         <v>170709.65814590399</v>
       </c>
       <c r="K40">
+        <f t="shared" si="0"/>
+        <v>125799.67578069448</v>
+      </c>
+      <c r="L40">
         <f t="shared" si="1"/>
-        <v>125552.7627468108</v>
-      </c>
-      <c r="L40">
-        <f t="shared" si="0"/>
-        <v>125.5527627468108</v>
+        <v>125.79967578069449</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
@@ -19038,12 +19059,12 @@
         <v>520997.73669242801</v>
       </c>
       <c r="K44">
+        <f t="shared" si="0"/>
+        <v>533115.93206540786</v>
+      </c>
+      <c r="L44">
         <f t="shared" si="1"/>
-        <v>532561.01465225173</v>
-      </c>
-      <c r="L44">
-        <f t="shared" si="0"/>
-        <v>532.56101465225174</v>
+        <v>533.11593206540783</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
@@ -19078,12 +19099,12 @@
         <v>386747.41315841599</v>
       </c>
       <c r="K45">
+        <f t="shared" si="0"/>
+        <v>398366.26966611599</v>
+      </c>
+      <c r="L45">
         <f t="shared" si="1"/>
-        <v>397553.15136909438</v>
-      </c>
-      <c r="L45">
-        <f t="shared" si="0"/>
-        <v>397.55315136909439</v>
+        <v>398.36626966611601</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
@@ -19118,12 +19139,12 @@
         <v>319196.13051414402</v>
       </c>
       <c r="K46">
+        <f t="shared" si="0"/>
+        <v>334136.63776532898</v>
+      </c>
+      <c r="L46">
         <f t="shared" si="1"/>
-        <v>333567.68393516529</v>
-      </c>
-      <c r="L46">
-        <f t="shared" si="0"/>
-        <v>333.56768393516529</v>
+        <v>334.136637765329</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.3">
@@ -19158,12 +19179,12 @@
         <v>316463.77110481198</v>
       </c>
       <c r="K47">
+        <f t="shared" si="0"/>
+        <v>331369.01624814741</v>
+      </c>
+      <c r="L47">
         <f t="shared" si="1"/>
-        <v>330530.35879135114</v>
-      </c>
-      <c r="L47">
-        <f t="shared" si="0"/>
-        <v>330.53035879135115</v>
+        <v>331.36901624814743</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
@@ -19198,12 +19219,12 @@
         <v>324487.36715316703</v>
       </c>
       <c r="K48">
+        <f t="shared" si="0"/>
+        <v>339386.68759481126</v>
+      </c>
+      <c r="L48">
         <f t="shared" si="1"/>
-        <v>338572.91650772019</v>
-      </c>
-      <c r="L48">
-        <f t="shared" si="0"/>
-        <v>338.57291650772021</v>
+        <v>339.38668759481129</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
@@ -19238,12 +19259,12 @@
         <v>323237.31780052098</v>
       </c>
       <c r="K49">
+        <f t="shared" si="0"/>
+        <v>339818.34324018192</v>
+      </c>
+      <c r="L49">
         <f t="shared" si="1"/>
-        <v>339063.58551979007</v>
-      </c>
-      <c r="L49">
-        <f t="shared" si="0"/>
-        <v>339.06358551979008</v>
+        <v>339.81834324018195</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
@@ -19278,12 +19299,12 @@
         <v>259692.99697875901</v>
       </c>
       <c r="K50">
+        <f t="shared" si="0"/>
+        <v>130403.10724393609</v>
+      </c>
+      <c r="L50">
         <f t="shared" si="1"/>
-        <v>129904.5290946959</v>
-      </c>
-      <c r="L50">
-        <f t="shared" si="0"/>
-        <v>129.9045290946959</v>
+        <v>130.40310724393609</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
@@ -19318,12 +19339,12 @@
         <v>212043.03503036499</v>
       </c>
       <c r="K51">
+        <f t="shared" si="0"/>
+        <v>73280.472356240789</v>
+      </c>
+      <c r="L51">
         <f t="shared" si="1"/>
-        <v>72833.636283874395</v>
-      </c>
-      <c r="L51">
-        <f t="shared" si="0"/>
-        <v>72.833636283874398</v>
+        <v>73.280472356240793</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.3">
@@ -19358,12 +19379,12 @@
         <v>222543.01023483201</v>
       </c>
       <c r="K52">
+        <f t="shared" si="0"/>
+        <v>70546.929675500389</v>
+      </c>
+      <c r="L52">
         <f t="shared" si="1"/>
-        <v>70010.224103927409</v>
-      </c>
-      <c r="L52">
-        <f t="shared" si="0"/>
-        <v>70.010224103927413</v>
+        <v>70.546929675500394</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -19398,12 +19419,12 @@
         <v>310964.67399597098</v>
       </c>
       <c r="K53">
+        <f t="shared" si="0"/>
+        <v>69340.525227944891</v>
+      </c>
+      <c r="L53">
         <f t="shared" si="1"/>
-        <v>69724.192857742193</v>
-      </c>
-      <c r="L53">
-        <f t="shared" si="0"/>
-        <v>69.724192857742196</v>
+        <v>69.340525227944894</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.3">
@@ -19448,12 +19469,12 @@
         <v>139517.54665374701</v>
       </c>
       <c r="K56">
+        <f t="shared" si="0"/>
+        <v>164106.27015249018</v>
+      </c>
+      <c r="L56">
         <f t="shared" si="1"/>
-        <v>163633.87227058399</v>
-      </c>
-      <c r="L56">
-        <f t="shared" si="0"/>
-        <v>163.63387227058399</v>
+        <v>164.10627015249017</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.3">
@@ -19488,12 +19509,12 @@
         <v>29955.364704132</v>
       </c>
       <c r="K57">
+        <f t="shared" si="0"/>
+        <v>59449.155169885205</v>
+      </c>
+      <c r="L57">
         <f t="shared" si="1"/>
-        <v>59525.467395782318</v>
-      </c>
-      <c r="L57">
-        <f t="shared" si="0"/>
-        <v>59.525467395782321</v>
+        <v>59.449155169885209</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.3">
@@ -19528,12 +19549,12 @@
         <v>18412.2338294982</v>
       </c>
       <c r="K58">
+        <f t="shared" si="0"/>
+        <v>47987.84382955324</v>
+      </c>
+      <c r="L58">
         <f t="shared" si="1"/>
-        <v>48144.936561584451</v>
-      </c>
-      <c r="L58">
-        <f t="shared" si="0"/>
-        <v>48.144936561584451</v>
+        <v>47.987843829553242</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.3">
@@ -19568,12 +19589,12 @@
         <v>17698.052883148099</v>
       </c>
       <c r="K59">
+        <f t="shared" si="0"/>
+        <v>47262.526828210459</v>
+      </c>
+      <c r="L59">
         <f t="shared" si="1"/>
-        <v>48015.802621841372</v>
-      </c>
-      <c r="L59">
-        <f t="shared" si="0"/>
-        <v>48.015802621841374</v>
+        <v>47.262526828210461</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.3">
@@ -19608,12 +19629,12 @@
         <v>17903.647661209099</v>
       </c>
       <c r="K60">
+        <f t="shared" si="0"/>
+        <v>47387.438136499026</v>
+      </c>
+      <c r="L60">
         <f t="shared" si="1"/>
-        <v>47603.817701339642</v>
-      </c>
-      <c r="L60">
-        <f t="shared" si="0"/>
-        <v>47.603817701339644</v>
+        <v>47.387438136499028</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.3">
@@ -19648,12 +19669,12 @@
         <v>20717.008590698199</v>
       </c>
       <c r="K61">
+        <f t="shared" si="0"/>
+        <v>50270.334083001697</v>
+      </c>
+      <c r="L61">
         <f t="shared" si="1"/>
-        <v>50672.729253768804</v>
-      </c>
-      <c r="L61">
-        <f t="shared" si="0"/>
-        <v>50.672729253768807</v>
+        <v>50.2703340830017</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.3">
@@ -19718,12 +19739,12 @@
         <v>7708943.4971809303</v>
       </c>
       <c r="K68">
+        <f t="shared" ref="K67:K103" si="2">SUM($E$105,G68,H68)</f>
+        <v>7741245.0185598489</v>
+      </c>
+      <c r="L68">
         <f t="shared" si="1"/>
-        <v>7740695.036888117</v>
-      </c>
-      <c r="L68">
-        <f t="shared" si="0"/>
-        <v>7740.6950368881171</v>
+        <v>7741.2450185598491</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
@@ -19758,12 +19779,12 @@
         <v>788959.96928215004</v>
       </c>
       <c r="K69">
+        <f t="shared" si="2"/>
+        <v>821261.51450292289</v>
+      </c>
+      <c r="L69">
         <f t="shared" si="1"/>
-        <v>821691.89095497061</v>
-      </c>
-      <c r="L69">
-        <f t="shared" si="0"/>
-        <v>821.69189095497063</v>
+        <v>821.26151450292286</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
@@ -19798,12 +19819,12 @@
         <v>94629.777908325195</v>
       </c>
       <c r="K70">
+        <f t="shared" si="2"/>
+        <v>126931.32718221429</v>
+      </c>
+      <c r="L70">
         <f t="shared" si="1"/>
-        <v>127251.6441345214</v>
-      </c>
-      <c r="L70">
-        <f t="shared" si="0"/>
-        <v>127.2516441345214</v>
+        <v>126.93132718221429</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
@@ -19838,12 +19859,12 @@
         <v>31592.154741287199</v>
       </c>
       <c r="K71">
+        <f t="shared" si="2"/>
+        <v>63893.704968850689</v>
+      </c>
+      <c r="L71">
         <f t="shared" si="1"/>
-        <v>65354.906082153197</v>
-      </c>
-      <c r="L71">
-        <f t="shared" si="0"/>
-        <v>65.354906082153192</v>
+        <v>63.893704968850692</v>
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
@@ -19878,12 +19899,12 @@
         <v>26760.7460021972</v>
       </c>
       <c r="K72">
+        <f t="shared" si="2"/>
+        <v>59062.306958596688</v>
+      </c>
+      <c r="L72">
         <f t="shared" si="1"/>
-        <v>59265.196561813202</v>
-      </c>
-      <c r="L72">
-        <f t="shared" si="0"/>
-        <v>59.265196561813205</v>
+        <v>59.062306958596686</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
@@ -19918,12 +19939,12 @@
         <v>26238.908767700101</v>
       </c>
       <c r="K73">
+        <f t="shared" si="2"/>
+        <v>58540.425855081085</v>
+      </c>
+      <c r="L73">
         <f t="shared" si="1"/>
-        <v>59234.9448204039</v>
-      </c>
-      <c r="L73">
-        <f t="shared" si="0"/>
-        <v>59.234944820403904</v>
+        <v>58.540425855081082</v>
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.3">
@@ -19958,12 +19979,12 @@
         <v>268986.62471771199</v>
       </c>
       <c r="K74">
+        <f t="shared" si="2"/>
+        <v>270600.55955068354</v>
+      </c>
+      <c r="L74">
         <f t="shared" si="1"/>
-        <v>271324.1124153136</v>
-      </c>
-      <c r="L74">
-        <f t="shared" si="0"/>
-        <v>271.32411241531361</v>
+        <v>270.60055955068356</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.3">
@@ -19998,12 +20019,12 @@
         <v>179024.81222152701</v>
       </c>
       <c r="K75">
+        <f t="shared" si="2"/>
+        <v>182624.8069585959</v>
+      </c>
+      <c r="L75">
         <f t="shared" si="1"/>
-        <v>183385.06245612999</v>
-      </c>
-      <c r="L75">
-        <f t="shared" si="0"/>
-        <v>183.38506245612999</v>
+        <v>182.62480695859591</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
@@ -20038,12 +20059,12 @@
         <v>174190.36245345999</v>
       </c>
       <c r="K76">
+        <f t="shared" si="2"/>
+        <v>177775.66822187178</v>
+      </c>
+      <c r="L76">
         <f t="shared" si="1"/>
-        <v>177155.46202659578</v>
-      </c>
-      <c r="L76">
-        <f t="shared" si="0"/>
-        <v>177.15546202659579</v>
+        <v>177.77566822187177</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
@@ -20078,12 +20099,12 @@
         <v>173419.88658905</v>
       </c>
       <c r="K77">
+        <f t="shared" si="2"/>
+        <v>177048.4917940305</v>
+      </c>
+      <c r="L77">
         <f t="shared" si="1"/>
-        <v>176504.1289329525</v>
-      </c>
-      <c r="L77">
-        <f t="shared" si="0"/>
-        <v>176.50412893295251</v>
+        <v>177.0484917940305</v>
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.3">
@@ -20128,12 +20149,12 @@
         <v>184708.36734771699</v>
       </c>
       <c r="K80">
+        <f t="shared" si="2"/>
+        <v>188254.29137365101</v>
+      </c>
+      <c r="L80">
         <f t="shared" si="1"/>
-        <v>188780.80916404701</v>
-      </c>
-      <c r="L80">
-        <f t="shared" si="0"/>
-        <v>188.78080916404701</v>
+        <v>188.254291373651</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.3">
@@ -20168,12 +20189,12 @@
         <v>127856.252670288</v>
       </c>
       <c r="K81">
+        <f t="shared" si="2"/>
+        <v>131267.05272809748</v>
+      </c>
+      <c r="L81">
         <f t="shared" si="1"/>
-        <v>131461.96365356431</v>
-      </c>
-      <c r="L81">
-        <f t="shared" si="0"/>
-        <v>131.46196365356431</v>
+        <v>131.26705272809747</v>
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.3">
@@ -20208,12 +20229,12 @@
         <v>123572.316884994</v>
       </c>
       <c r="K82">
+        <f t="shared" si="2"/>
+        <v>126886.26487867118</v>
+      </c>
+      <c r="L82">
         <f t="shared" si="1"/>
-        <v>127639.8167610167</v>
-      </c>
-      <c r="L82">
-        <f t="shared" si="0"/>
-        <v>127.6398167610167</v>
+        <v>126.88626487867118</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
@@ -20263,12 +20284,12 @@
         <v>599213.89722824097</v>
       </c>
       <c r="K86">
+        <f t="shared" si="2"/>
+        <v>610117.18519345974</v>
+      </c>
+      <c r="L86">
         <f t="shared" si="1"/>
-        <v>610371.99640274001</v>
-      </c>
-      <c r="L86">
-        <f t="shared" si="0"/>
-        <v>610.37199640274002</v>
+        <v>610.1171851934597</v>
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
@@ -20303,12 +20324,12 @@
         <v>386308.79306793201</v>
       </c>
       <c r="K87">
+        <f t="shared" si="2"/>
+        <v>396614.27004949289</v>
+      </c>
+      <c r="L87">
         <f t="shared" si="1"/>
-        <v>396046.00763320859</v>
-      </c>
-      <c r="L87">
-        <f t="shared" si="0"/>
-        <v>396.0460076332086</v>
+        <v>396.61427004949292</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
@@ -20343,12 +20364,12 @@
         <v>336028.19609642</v>
       </c>
       <c r="K88">
+        <f t="shared" si="2"/>
+        <v>342909.54692975734</v>
+      </c>
+      <c r="L88">
         <f t="shared" si="1"/>
-        <v>342633.03995132406</v>
-      </c>
-      <c r="L88">
-        <f t="shared" si="0"/>
-        <v>342.63303995132406</v>
+        <v>342.90954692975737</v>
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
@@ -20383,12 +20404,12 @@
         <v>320810.71853637602</v>
       </c>
       <c r="K89">
+        <f t="shared" si="2"/>
+        <v>338263.15172330616</v>
+      </c>
+      <c r="L89">
         <f t="shared" si="1"/>
-        <v>337772.59206771839</v>
-      </c>
-      <c r="L89">
-        <f t="shared" si="0"/>
-        <v>337.77259206771839</v>
+        <v>338.26315172330618</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
@@ -20423,12 +20444,12 @@
         <v>338015.92779159499</v>
       </c>
       <c r="K90">
+        <f t="shared" si="2"/>
+        <v>348196.27769605326</v>
+      </c>
+      <c r="L90">
         <f t="shared" si="1"/>
-        <v>347616.53542518528</v>
-      </c>
-      <c r="L90">
-        <f t="shared" si="0"/>
-        <v>347.6165354251853</v>
+        <v>348.19627769605324</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
@@ -20463,12 +20484,12 @@
         <v>335830.82532882597</v>
       </c>
       <c r="K91">
+        <f t="shared" si="2"/>
+        <v>346573.99447576259</v>
+      </c>
+      <c r="L91">
         <f t="shared" si="1"/>
-        <v>345979.67362403829</v>
-      </c>
-      <c r="L91">
-        <f t="shared" si="0"/>
-        <v>345.9796736240383</v>
+        <v>346.57399447576262</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
@@ -20503,12 +20524,12 @@
         <v>164773.06246757499</v>
       </c>
       <c r="K92">
-        <f t="shared" si="1"/>
-        <v>130654.30593490589</v>
+        <f t="shared" si="2"/>
+        <v>131183.74593869929</v>
       </c>
       <c r="L92">
-        <f t="shared" ref="L92:L103" si="2">PRODUCT(K92,0.001)</f>
-        <v>130.65430593490589</v>
+        <f t="shared" ref="L92:L103" si="3">PRODUCT(K92,0.001)</f>
+        <v>131.18374593869927</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
@@ -20543,12 +20564,12 @@
         <v>117511.768817901</v>
       </c>
       <c r="K93">
-        <f t="shared" ref="K93:K103" si="3">SUM(E93,G93,H93)</f>
-        <v>73312.692165374596</v>
+        <f t="shared" si="2"/>
+        <v>73400.918561379891</v>
       </c>
       <c r="L93">
-        <f t="shared" si="2"/>
-        <v>73.3126921653746</v>
+        <f t="shared" si="3"/>
+        <v>73.400918561379896</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
@@ -20583,12 +20604,12 @@
         <v>125250.150203704</v>
       </c>
       <c r="K94">
+        <f t="shared" si="2"/>
+        <v>69760.532695214686</v>
+      </c>
+      <c r="L94">
         <f t="shared" si="3"/>
-        <v>69629.256010055295</v>
-      </c>
-      <c r="L94">
-        <f t="shared" si="2"/>
-        <v>69.6292560100553</v>
+        <v>69.760532695214692</v>
       </c>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.3">
@@ -20623,12 +20644,12 @@
         <v>216298.45309257499</v>
       </c>
       <c r="K95">
+        <f t="shared" si="2"/>
+        <v>69309.853869836283</v>
+      </c>
+      <c r="L95">
         <f t="shared" si="3"/>
-        <v>68829.155921935802</v>
-      </c>
-      <c r="L95">
-        <f t="shared" si="2"/>
-        <v>68.829155921935808</v>
+        <v>69.309853869836289</v>
       </c>
     </row>
     <row r="96" spans="1:12" x14ac:dyDescent="0.3">
@@ -20673,12 +20694,12 @@
         <v>157134.82356071399</v>
       </c>
       <c r="K98">
+        <f t="shared" si="2"/>
+        <v>181522.86751882249</v>
+      </c>
+      <c r="L98">
         <f t="shared" si="3"/>
-        <v>181021.83413505473</v>
-      </c>
-      <c r="L98">
-        <f t="shared" si="2"/>
-        <v>181.02183413505472</v>
+        <v>181.52286751882249</v>
       </c>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.3">
@@ -20713,12 +20734,12 @@
         <v>33616.097688674898</v>
       </c>
       <c r="K99">
+        <f t="shared" si="2"/>
+        <v>62813.394147317449</v>
+      </c>
+      <c r="L99">
         <f t="shared" si="3"/>
-        <v>63025.802373885963</v>
-      </c>
-      <c r="L99">
-        <f t="shared" si="2"/>
-        <v>63.025802373885966</v>
+        <v>62.813394147317453</v>
       </c>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.3">
@@ -20753,12 +20774,12 @@
         <v>25787.0182991027</v>
       </c>
       <c r="K100">
+        <f t="shared" si="2"/>
+        <v>54939.173537652583</v>
+      </c>
+      <c r="L100">
         <f t="shared" si="3"/>
-        <v>55264.179706573399</v>
-      </c>
-      <c r="L100">
-        <f t="shared" si="2"/>
-        <v>55.264179706573401</v>
+        <v>54.939173537652586</v>
       </c>
     </row>
     <row r="101" spans="1:12" x14ac:dyDescent="0.3">
@@ -20793,12 +20814,12 @@
         <v>26448.655128479</v>
       </c>
       <c r="K101">
+        <f t="shared" si="2"/>
+        <v>55698.743659417698</v>
+      </c>
+      <c r="L101">
         <f t="shared" si="3"/>
-        <v>55869.282960891614</v>
-      </c>
-      <c r="L101">
-        <f t="shared" si="2"/>
-        <v>55.869282960891617</v>
+        <v>55.698743659417701</v>
       </c>
     </row>
     <row r="102" spans="1:12" x14ac:dyDescent="0.3">
@@ -20833,12 +20854,12 @@
         <v>28443.382024765</v>
       </c>
       <c r="K102">
+        <f t="shared" si="2"/>
+        <v>57695.400554101558</v>
+      </c>
+      <c r="L102">
         <f t="shared" si="3"/>
-        <v>58453.414440154978</v>
-      </c>
-      <c r="L102">
-        <f t="shared" si="2"/>
-        <v>58.45341444015498</v>
+        <v>57.69540055410156</v>
       </c>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.3">
@@ -20873,12 +20894,21 @@
         <v>30375.0338554382</v>
       </c>
       <c r="K103">
+        <f t="shared" si="2"/>
+        <v>59571.528750817815</v>
+      </c>
+      <c r="L103">
         <f t="shared" si="3"/>
-        <v>60051.828384399327</v>
-      </c>
-      <c r="L103">
-        <f t="shared" si="2"/>
-        <v>60.051828384399329</v>
+        <v>59.571528750817819</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D105" t="s">
+        <v>31</v>
+      </c>
+      <c r="E105">
+        <f>'10_trees'!E105</f>
+        <v>32303.568440835588</v>
       </c>
     </row>
   </sheetData>
@@ -20914,8 +20944,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C017CB98-5B48-43D2-A10D-785A512351D9}">
   <dimension ref="A1:R21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J58" sqref="J58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20963,19 +20993,19 @@
       </c>
       <c r="B3" s="1">
         <f>MIN('10_trees'!L2:'10_trees'!L7)</f>
-        <v>46.588900089263817</v>
+        <v>46.337956744592212</v>
       </c>
       <c r="C3" s="1">
         <f>MIN('10_trees'!L8:'10_trees'!L13)</f>
-        <v>46.957735776901124</v>
+        <v>46.727786857049516</v>
       </c>
       <c r="D3" s="1">
         <f>MIN('10_trees'!L20:'10_trees'!L25)</f>
-        <v>45.945363283157256</v>
+        <v>45.942891198556445</v>
       </c>
       <c r="E3" s="1">
         <f>MIN('10_trees'!L26:'10_trees'!L31)</f>
-        <v>44.644665479660013</v>
+        <v>44.458604413430805</v>
       </c>
       <c r="H3">
         <v>60.7</v>
@@ -21006,19 +21036,19 @@
       </c>
       <c r="B4" s="1">
         <f>MIN('500_trees'!L2:'500_trees'!L7)</f>
-        <v>87.255288362502895</v>
+        <v>86.640738088052302</v>
       </c>
       <c r="C4" s="1">
         <f>MIN('500_trees'!L8:'500_trees'!L13)</f>
-        <v>71.86143803596481</v>
+        <v>71.659197884957791</v>
       </c>
       <c r="D4" s="1">
         <f>MIN('500_trees'!L20:'500_trees'!L25)</f>
-        <v>53.451896667480419</v>
+        <v>53.154491740625012</v>
       </c>
       <c r="E4" s="1">
         <f>MIN('500_trees'!L26:'500_trees'!L31)</f>
-        <v>45.118538618087669</v>
+        <v>45.215932208459478</v>
       </c>
       <c r="H4">
         <v>146.19999999999999</v>
@@ -21049,19 +21079,19 @@
       </c>
       <c r="B5" s="1">
         <f>MIN('1600_trees'!L2:'1600_trees'!L7)</f>
-        <v>178.33080959320031</v>
+        <v>178.3245092214749</v>
       </c>
       <c r="C5" s="1">
         <f>MIN('1600_trees'!L8:'1600_trees'!L13)</f>
-        <v>127.31808519363391</v>
+        <v>127.19957955495599</v>
       </c>
       <c r="D5" s="1">
         <f>MIN('1600_trees'!L20:'1600_trees'!L25)</f>
-        <v>72.432852029800202</v>
+        <v>72.36979134694819</v>
       </c>
       <c r="E5" s="1">
         <f>MIN('1600_trees'!L28:'1600_trees'!L33)</f>
-        <v>57.542337894439626</v>
+        <v>57.993606406610112</v>
       </c>
       <c r="H5">
         <v>305.5</v>
@@ -21135,24 +21165,24 @@
       </c>
       <c r="B9" s="1">
         <f>MIN('10_trees'!L32:'10_trees'!L37)</f>
-        <v>45.822473049163719</v>
+        <v>46.461994248788429</v>
       </c>
       <c r="C9" s="1">
         <f>MIN('10_trees'!L38:'10_trees'!L43)</f>
-        <v>46.728768348693684</v>
+        <v>46.581592399041675</v>
       </c>
       <c r="D9" s="1">
         <f>MIN('10_trees'!L50:'10_trees'!L55)</f>
-        <v>45.9850335121154</v>
+        <v>46.214565116326888</v>
       </c>
       <c r="E9" s="1">
         <f>MIN('10_trees'!L56:'10_trees'!L61)</f>
-        <v>43.574426651000877</v>
+        <v>44.141585904519673</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="1">
         <f>MIN('10_trees'!L68:'10_trees'!L73)</f>
-        <v>49.247249603271371</v>
+        <v>49.288450557153269</v>
       </c>
       <c r="H9">
         <v>59.2</v>
@@ -21188,24 +21218,24 @@
       </c>
       <c r="B10" s="1">
         <f>MIN('500_trees'!L32:'500_trees'!L37)</f>
-        <v>85.755883693694898</v>
+        <v>86.128751832406479</v>
       </c>
       <c r="C10" s="1">
         <f>MIN('500_trees'!L38:'500_trees'!L43)</f>
-        <v>72.449626445770107</v>
+        <v>71.787981826226698</v>
       </c>
       <c r="D10" s="1">
         <f>MIN('500_trees'!L50:'500_trees'!L55)</f>
-        <v>52.779498338699256</v>
+        <v>52.620731192987037</v>
       </c>
       <c r="E10" s="1">
         <f>MIN('500_trees'!L56:'500_trees'!L61)</f>
-        <v>43.132436513900679</v>
+        <v>43.034369307916272</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="1">
         <f>MIN('500_trees'!L68:'500_trees'!L73)</f>
-        <v>53.278722286224301</v>
+        <v>53.245069819848602</v>
       </c>
       <c r="H10">
         <v>137.80000000000001</v>
@@ -21241,24 +21271,24 @@
       </c>
       <c r="B11" s="1">
         <f>MIN('1600_trees'!L32:'1600_trees'!L37)</f>
-        <v>176.60673642158417</v>
+        <v>176.6493080438774</v>
       </c>
       <c r="C11" s="1">
         <f>MIN('1600_trees'!L38:'1600_trees'!L43)</f>
-        <v>125.5527627468108</v>
+        <v>125.79967578069449</v>
       </c>
       <c r="D11" s="1">
         <f>MIN('1600_trees'!L50:'1600_trees'!L55)</f>
-        <v>69.724192857742196</v>
+        <v>69.340525227944894</v>
       </c>
       <c r="E11" s="1">
         <f>MIN('1600_trees'!L56:'1600_trees'!L61)</f>
-        <v>47.603817701339644</v>
+        <v>47.262526828210461</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1">
         <f>MIN('1600_trees'!L68:'1600_trees'!L73)</f>
-        <v>59.234944820403904</v>
+        <v>58.540425855081082</v>
       </c>
       <c r="H11">
         <v>287.10000000000002</v>
@@ -21331,19 +21361,19 @@
       </c>
       <c r="B15" s="1">
         <f>MIN('10_trees'!L74:'10_trees'!L79)</f>
-        <v>45.443762540817097</v>
+        <v>46.245139199655085</v>
       </c>
       <c r="C15" s="1">
         <f>MIN('10_trees'!L80:'10_trees'!L85)</f>
-        <v>46.475845575332549</v>
+        <v>46.370733577172842</v>
       </c>
       <c r="D15" s="1">
         <f>MIN('10_trees'!L92:'10_trees'!L97)</f>
-        <v>45.567111015319696</v>
+        <v>46.223801452081275</v>
       </c>
       <c r="E15" s="1">
         <f>MIN('10_trees'!L98:'10_trees'!L103)</f>
-        <v>42.292098522186251</v>
+        <v>42.219190198342915</v>
       </c>
       <c r="H15">
         <v>58.8</v>
@@ -21374,19 +21404,19 @@
       </c>
       <c r="B16" s="1">
         <f>MIN('500_trees'!L74:'500_trees'!L79)</f>
-        <v>85.861827135085903</v>
+        <v>86.201553183953791</v>
       </c>
       <c r="C16" s="1">
         <f>MIN('500_trees'!L80:'500_trees'!L85)</f>
-        <v>73.0877263545988</v>
+        <v>72.195126372735487</v>
       </c>
       <c r="D16" s="1">
         <f>MIN('500_trees'!L92:'500_trees'!L97)</f>
-        <v>53.220368623733449</v>
+        <v>52.516989308755441</v>
       </c>
       <c r="E16" s="1">
         <f>MIN('500_trees'!L98:'500_trees'!L103)</f>
-        <v>45.928158044815014</v>
+        <v>45.447910148065205</v>
       </c>
       <c r="H16">
         <v>98.8</v>
@@ -21417,19 +21447,19 @@
       </c>
       <c r="B17" s="1">
         <f>MIN('1600_trees'!L74:'1600_trees'!L79)</f>
-        <v>176.50412893295251</v>
+        <v>177.0484917940305</v>
       </c>
       <c r="C17" s="1">
         <f>MIN('1600_trees'!L80:'1600_trees'!L85)</f>
-        <v>127.6398167610167</v>
+        <v>126.88626487867118</v>
       </c>
       <c r="D17" s="1">
         <f>MIN('1600_trees'!L92:'1600_trees'!L97)</f>
-        <v>68.829155921935808</v>
+        <v>69.309853869836289</v>
       </c>
       <c r="E17" s="1">
         <f>MIN('1600_trees'!L98:'1600_trees'!L103)</f>
-        <v>55.264179706573401</v>
+        <v>54.939173537652586</v>
       </c>
       <c r="H17">
         <v>185</v>

</xml_diff>